<commit_message>
Changed wifi materials to match form
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sparrowdscom-my.sharepoint.com/personal/kevin_sparrowds_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C501610D-CB4A-4D88-96F3-A7E055BADCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{3B96DE0D-663C-4E09-A934-24E7DCDDABAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{693A055B-8CEC-411E-91F8-C7141F3EFD2D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="813" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27007" yWindow="2459" windowWidth="25159" windowHeight="17973" tabRatio="813" firstSheet="14" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -36,14 +36,17 @@
     <sheet name="Go_Build_Love" sheetId="17" r:id="rId21"/>
     <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId22"/>
     <sheet name="Serve_Hope" sheetId="21" r:id="rId23"/>
-    <sheet name="WiFi_Languages" sheetId="33" r:id="rId24"/>
-    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId25"/>
-    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId26"/>
+    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId24"/>
+    <sheet name="Wifi_Materials" sheetId="37" r:id="rId25"/>
+    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId26"/>
+    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId27"/>
+    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId28"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId27"/>
+    <externalReference r:id="rId29"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
     <definedName name="Reserved" localSheetId="20">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="21">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="22">[1]!tblReserved[Reserved keywords]</definedName>
@@ -76,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3534" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4176" uniqueCount="887">
   <si>
     <t>Latitude</t>
   </si>
@@ -2533,13 +2536,218 @@
   </si>
   <si>
     <t>Lumasaba</t>
+  </si>
+  <si>
+    <t>Material Name</t>
+  </si>
+  <si>
+    <t>Bible App</t>
+  </si>
+  <si>
+    <t>Jesus Film(s)</t>
+  </si>
+  <si>
+    <t>Bible Project Video(s)</t>
+  </si>
+  <si>
+    <t>Sawyer Cleaning Instructions</t>
+  </si>
+  <si>
+    <t>iBIBLE</t>
+  </si>
+  <si>
+    <t>Org Access</t>
+  </si>
+  <si>
+    <t>Languages Available</t>
+  </si>
+  <si>
+    <t>Acholi, Adele, Akan-Akuapem-Twi, Akan-Asante, Akan-Fante, Alur, Anufo, Apalai, Apinaye, Apurina, Ateso, Bakairi, Bekwarra, Berom, Bete-Bendi, Bimoba, Birifor-Southern, Bisa, Bokobaru-Sim, Borana, Bororo, Buli, Bura, Busa-Bisa, Canela, Canela, Chumburung, Culina, Daasanach, Dagaare, Dagbani, Dhopadhola, Duruma, Dza, Ebira, Embu, Ewe, Frafra, Ga, Gikyode, Giryama, Guajajara, Hanga, Hausa, Hixkaryana, Ilchamus, Jamamadi, Jarawara, Kaapor, Kadiweu, Kaingang, Kaiwa, Kakwa, Kalenjin, Kamayura, Kamba, Karaja, Karimojong, Kasem, Kayabi, Kayapo, Kebu, Kikuyu, Kisii, Kiswahili, Kiwilwana, Koma, Konkomba-Likoonli, Konkomba-Likpakpaaln, Kulina, Kumam, Kupsapiny, Kusaal, Lango, Lelemi, Lubukusu, Lubwisi, Luganda, Lugbara, Lugungu, Lugwere, Luhya, Lukakamega, Lumasaaba, Lunyore, Luo, Lusamya, Lusoga, Maasai, Macushi, Madi, Mampruli, Manchineri, Marakwet, Maxakali, Mbya Guarani, Meru, Munduruku, Nadeb, Nambikuara (Southern), Nawuri, Nkonya, Ntrubo, Nzema, Obolo, Okphela, Orma, Paasaal, Palikur, Parecis, Paumari, Pokoot, Portuguese, Rikbaktsa, Runyankore, Runyoro-Rutoro, Sabaot, Samburu, Satere-Mawe, Sekpele, Selee, Shanga, Sisaala-Tumulung, Siwu, Suba, Taita, Tampulma, Tenharim, Terena, Tharaka, Tiv, Tukano, Turkana, Tuwuli, Tyap, UaiUai, Vagla, Wali, Xavante, Yoruba,</t>
+  </si>
+  <si>
+    <t>English,</t>
+  </si>
+  <si>
+    <t>Spanish,</t>
+  </si>
+  <si>
+    <t>Portuguese,</t>
+  </si>
+  <si>
+    <t>Acholi, Adele, Akan-Akuapem-Twi, Akan-Asante, Akan-Fante, Alur, Anufo, Ateso, Bimoba, Birifor-Southern, Borana, Buli, Canela, Chumburung, Daasanach, Dagaare, Dagbani, Dhopadhola, Duruma, English, Ewe, Ga, Gikyode, Giryama, Guajajara, Hanga, Ilchamus, Kaapor, Kadiweu, Kakwa, Kalenjin, Kamba, Karimojong, Kasem, Kayabi, Kayapo, Kebu, Kiswahili, Kiwilwana, Koma, Konkomba-Likoonli, Konkomba-Likpakpaaln, Kumam, Kupsapiny, Kusaal, Lango, Lelemi, Lubwisi, Luganda, Lugbara, Lumasaaba, Lunyore, Luo, Lusoga, Maasai, Madi, Mampruli, Meru, Nkonya, Nzema, Paasaal, Parecis, Pokoot, Portuguese, Runyankore, Runyoro-Rutoro, Sabaot, Samburu, Sisaala-Tumulung, Spanish, Suba, Taita, Tampulma, Tharaka, Turkana, Vagla, Wali,</t>
+  </si>
+  <si>
+    <t>English, Kiswahili, Portuguese, Spanish,</t>
+  </si>
+  <si>
+    <t>Spanish, English,</t>
+  </si>
+  <si>
+    <t>Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, Baniwa, Banjara, Bengali, Bono, Bora, Buji, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, IsiXhosa, IsiZulu, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Konkomba, Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lumasaba, Lunyankore, Lusamya, Luyole, Magogo, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nchumburu, Ngas, Nhengatu, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sesotho, Sisaali, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
+  </si>
+  <si>
+    <t>TBM, TBMAR, TBMCV, TBMKA, TBMK,</t>
+  </si>
+  <si>
+    <t>TBM, TBMCV, TBMKA, TBMK,</t>
+  </si>
+  <si>
+    <t>TBM, TBMCV, TBMK,</t>
+  </si>
+  <si>
+    <t>TBM,</t>
+  </si>
+  <si>
+    <t>Language Not Available on WiFi Box
+Please notify Randy and Victor to update form and leave a note at the bottom of the form.</t>
+  </si>
+  <si>
+    <t>Download Name</t>
+  </si>
+  <si>
+    <t>Biblical Themes-Water of Life</t>
+  </si>
+  <si>
+    <t>Biblical Themes-God</t>
+  </si>
+  <si>
+    <t>Biblical Themes-Day of the Lord</t>
+  </si>
+  <si>
+    <t>Biblical Themes-Exile</t>
+  </si>
+  <si>
+    <t>Biblical Themes-Son of Man</t>
+  </si>
+  <si>
+    <t>Biblical Themes-The last will be first</t>
+  </si>
+  <si>
+    <t>Biblical Themes-Temple</t>
+  </si>
+  <si>
+    <t>Character of God-Loyal Love</t>
+  </si>
+  <si>
+    <t>Character of God-Compassion</t>
+  </si>
+  <si>
+    <t>Character of God-Faithfulness</t>
+  </si>
+  <si>
+    <t>Character of God-Grace</t>
+  </si>
+  <si>
+    <t>Character of God-The Character of God</t>
+  </si>
+  <si>
+    <t>Character of God-Slow to Anger</t>
+  </si>
+  <si>
+    <t>Heaven and Earth</t>
+  </si>
+  <si>
+    <t>How to Read Biblical Discourse-The Biblical Law</t>
+  </si>
+  <si>
+    <t>How to Read Biblical Discourse-NT Historical Context</t>
+  </si>
+  <si>
+    <t>How to Read Biblical Discourse-NT Literary Context</t>
+  </si>
+  <si>
+    <t>Word Study-Witness</t>
+  </si>
+  <si>
+    <t>Gospel of the Kingdom</t>
+  </si>
+  <si>
+    <t>Negative Words Series-Iniquity</t>
+  </si>
+  <si>
+    <t>Negative Words Series-Sin</t>
+  </si>
+  <si>
+    <t>Negative Words Series-Transgression</t>
+  </si>
+  <si>
+    <t>Shema Series-Love</t>
+  </si>
+  <si>
+    <t>Genisis Ch1: Creation</t>
+  </si>
+  <si>
+    <t>Download Category</t>
+  </si>
+  <si>
+    <t>bibleProject</t>
+  </si>
+  <si>
+    <t>cleaningInstructions</t>
+  </si>
+  <si>
+    <t>jesusFilm</t>
+  </si>
+  <si>
+    <t>Kiswahili,</t>
+  </si>
+  <si>
+    <t>Spanish, Portuguese,</t>
+  </si>
+  <si>
+    <t>Spanish, Kiswahili, Portuguese,</t>
+  </si>
+  <si>
+    <t>Kiswahili, Portuguese,</t>
+  </si>
+  <si>
+    <t>Spanish, English, Kiswahili,</t>
+  </si>
+  <si>
+    <t>Spanish, English, Portuguese,</t>
+  </si>
+  <si>
+    <t>Acholi, Adele, Akan-Akuapem-Twi, Akan-Asante, Akan-Fante, Alur, Anufo, Ateso, Bimoba, Birifor-Southern, Borana, Buli, Canela, Chumburung, Daasanach, Dagaare, Dagbani, Dhopadhola, Duruma, English, Ewe, Ga, Gikyode, Giryama, Guajajara, Hanga, Ilchamus, Kaapor, Kadiweu, Kakwa, Kalenjin, Kamba, Karimojong, Kasem, Kayabi, Kayapo,  Kebu, Kikamba, Kimeru, Kiswahili, Kiwihwana, Koma, Konkomba-Likoonli, Konkomba-Likpakpaaln, Kumam, Kupsapiny, Kusaal, Lango, Lelemi, Lubwisi, Luganda, Lugbara, Lumasaaba, Lunyore, Luo, Lusoga, Maasai, Madi, Mampruli, Meru, Nkonya, Nzema, Paasaal, Parecis, Polkoot, Portuguese, Runyankore, Runyoro-Rutoro, Sabaot, Samburu, Sisaala-Tumulung, Spanish, Suba, Taita, Tampulma, Tharaka, Turkana, Vagla, Wali,</t>
+  </si>
+  <si>
+    <t>Maasai, Suba, Portuguese,</t>
+  </si>
+  <si>
+    <t>Acholi, Akan-Akuapem-Twi, Akan-Asante, Anufo, Dagbani, English, Ewe, Kasem, Kiswahili, Konkomba-Likoonli, Konkomba-Likpakpaaln, Kusaal, Luganda, Runyankore, Sisaala-Tumulung,</t>
+  </si>
+  <si>
+    <t>Akan-Akuapem-Twi, English, Kiswahili, Portuguese,</t>
+  </si>
+  <si>
+    <t>Akan-Akuapem-Twi, Akan-Asante, English, Portuguese,</t>
+  </si>
+  <si>
+    <t>Akan-Akuapem-Twi, Akan-Asante, Ewe, Kiswahili, Luganda, Portuguese,</t>
+  </si>
+  <si>
+    <t>Akan-Asante, Kiswahili, Luganda, Portuguese,</t>
+  </si>
+  <si>
+    <t>Canela, Guajajara, Kaapor, Kadiweu, Kayabi, Kayapo, Parecis,</t>
+  </si>
+  <si>
+    <t>English, Kiswahili, Portuguese,</t>
+  </si>
+  <si>
+    <t>English, Portuguese,</t>
+  </si>
+  <si>
+    <t>English, Kiswahili,</t>
+  </si>
+  <si>
+    <t>Ewe, Kiswahili,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2708,6 +2916,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2744,7 +2960,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2803,13 +3019,19 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="16" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2817,7 +3039,28 @@
     <cellStyle name="Normal 3" xfId="2" xr:uid="{C6976ACF-4CF3-445D-A0DA-B78AF634B62B}"/>
     <cellStyle name="Normal 3 2" xfId="3" xr:uid="{7CE6C237-AEFB-4568-BA38-55AF6AE605BA}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
@@ -3241,24 +3484,24 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
@@ -3419,23 +3662,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
@@ -3964,23 +4207,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -4266,9 +4509,9 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4276,12 +4519,12 @@
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -4508,11 +4751,11 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4521,12 +4764,12 @@
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="19" t="s">
         <v>507</v>
       </c>
@@ -4608,23 +4851,23 @@
       <selection activeCell="D11" sqref="D11:D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -4928,28 +5171,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00598E5C-D8DC-4176-B37C-0365BB6BC78A}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>407</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5188,24 +5431,24 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5369,24 +5612,24 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>409</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5753,22 +5996,22 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="38" t="s">
         <v>413</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5878,24 +6121,24 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>410</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6071,23 +6314,23 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6247,22 +6490,22 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>412</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6383,23 +6626,23 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6559,9 +6802,9 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6569,12 +6812,12 @@
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>411</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6734,23 +6977,23 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6906,15 +7149,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}">
   <dimension ref="A1:D636"/>
   <sheetViews>
-    <sheetView topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="A380" sqref="A380"/>
+    <sheetView topLeftCell="A604" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="20.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -6932,13 +7175,13 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="34" t="s">
         <v>558</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C2" s="36" t="s">
+      <c r="B2" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D2" t="s">
@@ -7716,13 +7959,13 @@
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="34" t="s">
         <v>559</v>
       </c>
-      <c r="B58" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C58" s="36" t="s">
+      <c r="B58" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C58" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D58" t="s">
@@ -7884,13 +8127,13 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="36" t="s">
+      <c r="A70" s="34" t="s">
         <v>560</v>
       </c>
-      <c r="B70" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C70" s="36" t="s">
+      <c r="B70" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C70" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D70" t="s">
@@ -7898,13 +8141,13 @@
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="36" t="s">
+      <c r="A71" s="34" t="s">
         <v>560</v>
       </c>
-      <c r="B71" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C71" s="36" t="s">
+      <c r="B71" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C71" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D71" t="s">
@@ -8416,13 +8659,13 @@
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" s="36" t="s">
+      <c r="A108" s="34" t="s">
         <v>561</v>
       </c>
-      <c r="B108" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C108" s="36" t="s">
+      <c r="B108" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C108" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D108" t="s">
@@ -8430,13 +8673,13 @@
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" s="36" t="s">
+      <c r="A109" s="34" t="s">
         <v>561</v>
       </c>
-      <c r="B109" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C109" s="36" t="s">
+      <c r="B109" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C109" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D109" t="s">
@@ -10488,13 +10731,13 @@
       </c>
     </row>
     <row r="256" spans="1:4">
-      <c r="A256" s="36" t="s">
+      <c r="A256" s="34" t="s">
         <v>562</v>
       </c>
-      <c r="B256" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C256" s="36" t="s">
+      <c r="B256" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C256" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D256" t="s">
@@ -10502,13 +10745,13 @@
       </c>
     </row>
     <row r="257" spans="1:4">
-      <c r="A257" s="36" t="s">
+      <c r="A257" s="34" t="s">
         <v>562</v>
       </c>
-      <c r="B257" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C257" s="36" t="s">
+      <c r="B257" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C257" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D257" t="s">
@@ -12210,13 +12453,13 @@
       </c>
     </row>
     <row r="379" spans="1:4">
-      <c r="A379" s="36" t="s">
+      <c r="A379" s="34" t="s">
         <v>568</v>
       </c>
-      <c r="B379" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C379" s="36" t="s">
+      <c r="B379" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C379" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D379" t="s">
@@ -12238,13 +12481,13 @@
       </c>
     </row>
     <row r="381" spans="1:4">
-      <c r="A381" s="36" t="s">
+      <c r="A381" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B381" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C381" s="36" t="s">
+      <c r="B381" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C381" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D381" t="s">
@@ -12252,13 +12495,13 @@
       </c>
     </row>
     <row r="382" spans="1:4">
-      <c r="A382" s="36" t="s">
+      <c r="A382" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B382" s="36" t="s">
+      <c r="B382" s="34" t="s">
         <v>637</v>
       </c>
-      <c r="C382" s="36" t="s">
+      <c r="C382" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D382" t="s">
@@ -12266,13 +12509,13 @@
       </c>
     </row>
     <row r="383" spans="1:4">
-      <c r="A383" s="36" t="s">
+      <c r="A383" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B383" s="36" t="s">
+      <c r="B383" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="C383" s="36" t="s">
+      <c r="C383" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D383" t="s">
@@ -12280,13 +12523,13 @@
       </c>
     </row>
     <row r="384" spans="1:4">
-      <c r="A384" s="36" t="s">
+      <c r="A384" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B384" s="36" t="s">
+      <c r="B384" s="34" t="s">
         <v>609</v>
       </c>
-      <c r="C384" s="36" t="s">
+      <c r="C384" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D384" t="s">
@@ -12294,13 +12537,13 @@
       </c>
     </row>
     <row r="385" spans="1:4">
-      <c r="A385" s="36" t="s">
+      <c r="A385" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B385" s="36" t="s">
+      <c r="B385" s="34" t="s">
         <v>610</v>
       </c>
-      <c r="C385" s="36" t="s">
+      <c r="C385" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D385" t="s">
@@ -12322,13 +12565,13 @@
       </c>
     </row>
     <row r="387" spans="1:4">
-      <c r="A387" s="36" t="s">
+      <c r="A387" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B387" s="36" t="s">
+      <c r="B387" s="34" t="s">
         <v>612</v>
       </c>
-      <c r="C387" s="36" t="s">
+      <c r="C387" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D387" t="s">
@@ -12350,13 +12593,13 @@
       </c>
     </row>
     <row r="389" spans="1:4">
-      <c r="A389" s="36" t="s">
+      <c r="A389" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B389" s="36" t="s">
+      <c r="B389" s="34" t="s">
         <v>614</v>
       </c>
-      <c r="C389" s="36" t="s">
+      <c r="C389" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D389" t="s">
@@ -12364,13 +12607,13 @@
       </c>
     </row>
     <row r="390" spans="1:4">
-      <c r="A390" s="36" t="s">
+      <c r="A390" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B390" s="36" t="s">
+      <c r="B390" s="34" t="s">
         <v>616</v>
       </c>
-      <c r="C390" s="36" t="s">
+      <c r="C390" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D390" t="s">
@@ -12378,13 +12621,13 @@
       </c>
     </row>
     <row r="391" spans="1:4">
-      <c r="A391" s="36" t="s">
+      <c r="A391" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B391" s="36" t="s">
+      <c r="B391" s="34" t="s">
         <v>615</v>
       </c>
-      <c r="C391" s="36" t="s">
+      <c r="C391" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D391" t="s">
@@ -12392,13 +12635,13 @@
       </c>
     </row>
     <row r="392" spans="1:4">
-      <c r="A392" s="36" t="s">
+      <c r="A392" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B392" s="36" t="s">
+      <c r="B392" s="34" t="s">
         <v>617</v>
       </c>
-      <c r="C392" s="36" t="s">
+      <c r="C392" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D392" t="s">
@@ -12420,13 +12663,13 @@
       </c>
     </row>
     <row r="394" spans="1:4">
-      <c r="A394" s="36" t="s">
+      <c r="A394" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B394" s="36" t="s">
+      <c r="B394" s="34" t="s">
         <v>619</v>
       </c>
-      <c r="C394" s="36" t="s">
+      <c r="C394" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D394" t="s">
@@ -12434,13 +12677,13 @@
       </c>
     </row>
     <row r="395" spans="1:4">
-      <c r="A395" s="36" t="s">
+      <c r="A395" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B395" s="36" t="s">
+      <c r="B395" s="34" t="s">
         <v>621</v>
       </c>
-      <c r="C395" s="36" t="s">
+      <c r="C395" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D395" t="s">
@@ -12448,13 +12691,13 @@
       </c>
     </row>
     <row r="396" spans="1:4">
-      <c r="A396" s="36" t="s">
+      <c r="A396" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B396" s="36" t="s">
+      <c r="B396" s="34" t="s">
         <v>622</v>
       </c>
-      <c r="C396" s="36" t="s">
+      <c r="C396" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D396" t="s">
@@ -12462,13 +12705,13 @@
       </c>
     </row>
     <row r="397" spans="1:4">
-      <c r="A397" s="36" t="s">
+      <c r="A397" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B397" s="36" t="s">
+      <c r="B397" s="34" t="s">
         <v>623</v>
       </c>
-      <c r="C397" s="36" t="s">
+      <c r="C397" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D397" t="s">
@@ -12504,13 +12747,13 @@
       </c>
     </row>
     <row r="400" spans="1:4">
-      <c r="A400" s="36" t="s">
+      <c r="A400" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B400" s="36" t="s">
+      <c r="B400" s="34" t="s">
         <v>626</v>
       </c>
-      <c r="C400" s="36" t="s">
+      <c r="C400" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D400" t="s">
@@ -12532,13 +12775,13 @@
       </c>
     </row>
     <row r="402" spans="1:4">
-      <c r="A402" s="36" t="s">
+      <c r="A402" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B402" s="36" t="s">
+      <c r="B402" s="34" t="s">
         <v>628</v>
       </c>
-      <c r="C402" s="36" t="s">
+      <c r="C402" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D402" t="s">
@@ -12546,13 +12789,13 @@
       </c>
     </row>
     <row r="403" spans="1:4">
-      <c r="A403" s="36" t="s">
+      <c r="A403" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B403" s="36" t="s">
+      <c r="B403" s="34" t="s">
         <v>629</v>
       </c>
-      <c r="C403" s="36" t="s">
+      <c r="C403" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D403" t="s">
@@ -12560,13 +12803,13 @@
       </c>
     </row>
     <row r="404" spans="1:4">
-      <c r="A404" s="36" t="s">
+      <c r="A404" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B404" s="36" t="s">
+      <c r="B404" s="34" t="s">
         <v>630</v>
       </c>
-      <c r="C404" s="36" t="s">
+      <c r="C404" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D404" t="s">
@@ -12574,13 +12817,13 @@
       </c>
     </row>
     <row r="405" spans="1:4">
-      <c r="A405" s="36" t="s">
+      <c r="A405" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B405" s="36" t="s">
+      <c r="B405" s="34" t="s">
         <v>631</v>
       </c>
-      <c r="C405" s="36" t="s">
+      <c r="C405" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D405" t="s">
@@ -12588,13 +12831,13 @@
       </c>
     </row>
     <row r="406" spans="1:4">
-      <c r="A406" s="36" t="s">
+      <c r="A406" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B406" s="36" t="s">
+      <c r="B406" s="34" t="s">
         <v>632</v>
       </c>
-      <c r="C406" s="36" t="s">
+      <c r="C406" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D406" t="s">
@@ -12602,13 +12845,13 @@
       </c>
     </row>
     <row r="407" spans="1:4">
-      <c r="A407" s="36" t="s">
+      <c r="A407" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="B407" s="36" t="s">
+      <c r="B407" s="34" t="s">
         <v>633</v>
       </c>
-      <c r="C407" s="36" t="s">
+      <c r="C407" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D407" t="s">
@@ -12616,13 +12859,13 @@
       </c>
     </row>
     <row r="408" spans="1:4">
-      <c r="A408" s="36" t="s">
+      <c r="A408" s="34" t="s">
         <v>570</v>
       </c>
-      <c r="B408" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C408" s="36" t="s">
+      <c r="B408" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C408" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D408" t="s">
@@ -12644,13 +12887,13 @@
       </c>
     </row>
     <row r="410" spans="1:4">
-      <c r="A410" s="36" t="s">
+      <c r="A410" s="34" t="s">
         <v>571</v>
       </c>
-      <c r="B410" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C410" s="36" t="s">
+      <c r="B410" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C410" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D410" t="s">
@@ -12658,13 +12901,13 @@
       </c>
     </row>
     <row r="411" spans="1:4">
-      <c r="A411" s="36" t="s">
+      <c r="A411" s="34" t="s">
         <v>572</v>
       </c>
-      <c r="B411" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C411" s="36" t="s">
+      <c r="B411" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C411" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D411" t="s">
@@ -12700,13 +12943,13 @@
       </c>
     </row>
     <row r="414" spans="1:4">
-      <c r="A414" s="36" t="s">
+      <c r="A414" s="34" t="s">
         <v>818</v>
       </c>
-      <c r="B414" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C414" s="36" t="s">
+      <c r="B414" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C414" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D414" t="s">
@@ -12714,13 +12957,13 @@
       </c>
     </row>
     <row r="415" spans="1:4">
-      <c r="A415" s="36" t="s">
+      <c r="A415" s="34" t="s">
         <v>818</v>
       </c>
-      <c r="B415" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C415" s="36" t="s">
+      <c r="B415" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C415" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D415" t="s">
@@ -12728,13 +12971,13 @@
       </c>
     </row>
     <row r="416" spans="1:4">
-      <c r="A416" s="36" t="s">
+      <c r="A416" s="34" t="s">
         <v>817</v>
       </c>
-      <c r="B416" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C416" s="36" t="s">
+      <c r="B416" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C416" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D416" t="s">
@@ -12784,13 +13027,13 @@
       </c>
     </row>
     <row r="420" spans="1:4">
-      <c r="A420" s="36" t="s">
+      <c r="A420" s="34" t="s">
         <v>574</v>
       </c>
-      <c r="B420" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C420" s="36" t="s">
+      <c r="B420" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C420" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D420" t="s">
@@ -12798,13 +13041,13 @@
       </c>
     </row>
     <row r="421" spans="1:4">
-      <c r="A421" s="36" t="s">
+      <c r="A421" s="34" t="s">
         <v>575</v>
       </c>
-      <c r="B421" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C421" s="36" t="s">
+      <c r="B421" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C421" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D421" t="s">
@@ -12812,13 +13055,13 @@
       </c>
     </row>
     <row r="422" spans="1:4">
-      <c r="A422" s="36" t="s">
+      <c r="A422" s="34" t="s">
         <v>575</v>
       </c>
-      <c r="B422" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C422" s="36" t="s">
+      <c r="B422" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C422" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D422" t="s">
@@ -14758,13 +15001,13 @@
       </c>
     </row>
     <row r="561" spans="1:4">
-      <c r="A561" s="36" t="s">
+      <c r="A561" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B561" s="36" t="s">
-        <v>421</v>
-      </c>
-      <c r="C561" s="36" t="s">
+      <c r="B561" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C561" s="34" t="s">
         <v>421</v>
       </c>
       <c r="D561" t="s">
@@ -14772,13 +15015,13 @@
       </c>
     </row>
     <row r="562" spans="1:4">
-      <c r="A562" s="36" t="s">
+      <c r="A562" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B562" s="36" t="s">
-        <v>446</v>
-      </c>
-      <c r="C562" s="36" t="s">
+      <c r="B562" s="34" t="s">
+        <v>446</v>
+      </c>
+      <c r="C562" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D562" t="s">
@@ -14786,13 +15029,13 @@
       </c>
     </row>
     <row r="563" spans="1:4">
-      <c r="A563" s="36" t="s">
+      <c r="A563" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B563" s="36" t="s">
+      <c r="B563" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="C563" s="36" t="s">
+      <c r="C563" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D563" t="s">
@@ -14800,13 +15043,13 @@
       </c>
     </row>
     <row r="564" spans="1:4">
-      <c r="A564" s="36" t="s">
+      <c r="A564" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B564" s="36" t="s">
+      <c r="B564" s="34" t="s">
         <v>609</v>
       </c>
-      <c r="C564" s="36" t="s">
+      <c r="C564" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D564" t="s">
@@ -14814,13 +15057,13 @@
       </c>
     </row>
     <row r="565" spans="1:4">
-      <c r="A565" s="36" t="s">
+      <c r="A565" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B565" s="36" t="s">
+      <c r="B565" s="34" t="s">
         <v>610</v>
       </c>
-      <c r="C565" s="36" t="s">
+      <c r="C565" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D565" t="s">
@@ -14828,13 +15071,13 @@
       </c>
     </row>
     <row r="566" spans="1:4">
-      <c r="A566" s="36" t="s">
+      <c r="A566" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B566" s="36" t="s">
+      <c r="B566" s="34" t="s">
         <v>611</v>
       </c>
-      <c r="C566" s="36" t="s">
+      <c r="C566" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D566" t="s">
@@ -14842,13 +15085,13 @@
       </c>
     </row>
     <row r="567" spans="1:4">
-      <c r="A567" s="36" t="s">
+      <c r="A567" s="34" t="s">
         <v>592</v>
       </c>
-      <c r="B567" s="36" t="s">
+      <c r="B567" s="34" t="s">
         <v>612</v>
       </c>
-      <c r="C567" s="36" t="s">
+      <c r="C567" s="34" t="s">
         <v>446</v>
       </c>
       <c r="D567" t="s">
@@ -15822,6 +16065,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D636" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C509">
     <sortCondition ref="A2:A509"/>
   </sortState>
@@ -15830,6 +16074,2415 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>819</v>
+      </c>
+      <c r="B1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="326.05">
+      <c r="A2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>835</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>836</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>837</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>837</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="23" t="s">
+        <v>509</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>837</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="23" t="s">
+        <v>510</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>837</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="195.65">
+      <c r="A8" t="s">
+        <v>821</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>835</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>822</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>835</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>487</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>835</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>823</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>835</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>824</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>838</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="260.85000000000002">
+      <c r="A13" s="36" t="s">
+        <v>839</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>835</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>834</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
+  <dimension ref="A1:C204"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C204"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B2" t="s">
+        <v>866</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B3" t="s">
+        <v>866</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B4" t="s">
+        <v>866</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>432</v>
+      </c>
+      <c r="B5" t="s">
+        <v>866</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>460</v>
+      </c>
+      <c r="B6" t="s">
+        <v>866</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>433</v>
+      </c>
+      <c r="B7" t="s">
+        <v>866</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>434</v>
+      </c>
+      <c r="B8" t="s">
+        <v>866</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>435</v>
+      </c>
+      <c r="B9" t="s">
+        <v>866</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" t="s">
+        <v>866</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>437</v>
+      </c>
+      <c r="B11" t="s">
+        <v>866</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>461</v>
+      </c>
+      <c r="B12" t="s">
+        <v>866</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>438</v>
+      </c>
+      <c r="B13" t="s">
+        <v>866</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>462</v>
+      </c>
+      <c r="B14" t="s">
+        <v>866</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>439</v>
+      </c>
+      <c r="B15" t="s">
+        <v>866</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>841</v>
+      </c>
+      <c r="B16" t="s">
+        <v>866</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>842</v>
+      </c>
+      <c r="B17" t="s">
+        <v>866</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>843</v>
+      </c>
+      <c r="B18" t="s">
+        <v>866</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>844</v>
+      </c>
+      <c r="B19" t="s">
+        <v>866</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>845</v>
+      </c>
+      <c r="B20" t="s">
+        <v>866</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>846</v>
+      </c>
+      <c r="B21" t="s">
+        <v>866</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>847</v>
+      </c>
+      <c r="B22" t="s">
+        <v>866</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>848</v>
+      </c>
+      <c r="B23" t="s">
+        <v>866</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>849</v>
+      </c>
+      <c r="B24" t="s">
+        <v>866</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>850</v>
+      </c>
+      <c r="B25" t="s">
+        <v>866</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>851</v>
+      </c>
+      <c r="B26" t="s">
+        <v>866</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>852</v>
+      </c>
+      <c r="B27" t="s">
+        <v>866</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>853</v>
+      </c>
+      <c r="B28" t="s">
+        <v>866</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>854</v>
+      </c>
+      <c r="B29" t="s">
+        <v>866</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>463</v>
+      </c>
+      <c r="B30" t="s">
+        <v>866</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>464</v>
+      </c>
+      <c r="B31" t="s">
+        <v>866</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>465</v>
+      </c>
+      <c r="B32" t="s">
+        <v>866</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>466</v>
+      </c>
+      <c r="B33" t="s">
+        <v>866</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>855</v>
+      </c>
+      <c r="B34" t="s">
+        <v>866</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>856</v>
+      </c>
+      <c r="B35" t="s">
+        <v>866</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>857</v>
+      </c>
+      <c r="B36" t="s">
+        <v>866</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>858</v>
+      </c>
+      <c r="B37" t="s">
+        <v>866</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>859</v>
+      </c>
+      <c r="B38" t="s">
+        <v>866</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>423</v>
+      </c>
+      <c r="B39" t="s">
+        <v>866</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>440</v>
+      </c>
+      <c r="B40" t="s">
+        <v>866</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>467</v>
+      </c>
+      <c r="B41" t="s">
+        <v>866</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>468</v>
+      </c>
+      <c r="B42" t="s">
+        <v>866</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>441</v>
+      </c>
+      <c r="B43" t="s">
+        <v>866</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>470</v>
+      </c>
+      <c r="B44" t="s">
+        <v>866</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>511</v>
+      </c>
+      <c r="B45" t="s">
+        <v>866</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>860</v>
+      </c>
+      <c r="B46" t="s">
+        <v>866</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>861</v>
+      </c>
+      <c r="B47" t="s">
+        <v>866</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>862</v>
+      </c>
+      <c r="B48" t="s">
+        <v>866</v>
+      </c>
+      <c r="C48" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>442</v>
+      </c>
+      <c r="B49" t="s">
+        <v>866</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>471</v>
+      </c>
+      <c r="B50" t="s">
+        <v>866</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>425</v>
+      </c>
+      <c r="B51" t="s">
+        <v>866</v>
+      </c>
+      <c r="C51" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>428</v>
+      </c>
+      <c r="B52" t="s">
+        <v>866</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>863</v>
+      </c>
+      <c r="B53" t="s">
+        <v>866</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>426</v>
+      </c>
+      <c r="B54" t="s">
+        <v>866</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>773</v>
+      </c>
+      <c r="B55" t="s">
+        <v>866</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>427</v>
+      </c>
+      <c r="B56" t="s">
+        <v>866</v>
+      </c>
+      <c r="C56" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>429</v>
+      </c>
+      <c r="B57" t="s">
+        <v>866</v>
+      </c>
+      <c r="C57" s="35" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>443</v>
+      </c>
+      <c r="B58" t="s">
+        <v>866</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>784</v>
+      </c>
+      <c r="B59" t="s">
+        <v>866</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>472</v>
+      </c>
+      <c r="B60" t="s">
+        <v>866</v>
+      </c>
+      <c r="C60" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>473</v>
+      </c>
+      <c r="B61" t="s">
+        <v>866</v>
+      </c>
+      <c r="C61" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>474</v>
+      </c>
+      <c r="B62" t="s">
+        <v>866</v>
+      </c>
+      <c r="C62" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>445</v>
+      </c>
+      <c r="B63" t="s">
+        <v>866</v>
+      </c>
+      <c r="C63" s="35" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>444</v>
+      </c>
+      <c r="B64" t="s">
+        <v>866</v>
+      </c>
+      <c r="C64" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="C65" s="35"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>447</v>
+      </c>
+      <c r="B66" t="s">
+        <v>867</v>
+      </c>
+      <c r="C66" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>449</v>
+      </c>
+      <c r="B67" t="s">
+        <v>867</v>
+      </c>
+      <c r="C67" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="C68" s="35"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>864</v>
+      </c>
+      <c r="B69" t="s">
+        <v>824</v>
+      </c>
+      <c r="C69" s="35" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="C70" s="35"/>
+    </row>
+    <row r="71" spans="1:3" ht="179.35">
+      <c r="A71" t="s">
+        <v>446</v>
+      </c>
+      <c r="B71" t="s">
+        <v>868</v>
+      </c>
+      <c r="C71" s="35" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>478</v>
+      </c>
+      <c r="B72" t="s">
+        <v>868</v>
+      </c>
+      <c r="C72" s="35" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="48.9">
+      <c r="A73" t="s">
+        <v>608</v>
+      </c>
+      <c r="B73" t="s">
+        <v>868</v>
+      </c>
+      <c r="C73" s="35" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="48.9">
+      <c r="A74" t="s">
+        <v>609</v>
+      </c>
+      <c r="B74" t="s">
+        <v>868</v>
+      </c>
+      <c r="C74" s="35" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="48.9">
+      <c r="A75" t="s">
+        <v>610</v>
+      </c>
+      <c r="B75" t="s">
+        <v>868</v>
+      </c>
+      <c r="C75" s="35" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="48.9">
+      <c r="A76" t="s">
+        <v>611</v>
+      </c>
+      <c r="B76" t="s">
+        <v>868</v>
+      </c>
+      <c r="C76" s="35" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="48.9">
+      <c r="A77" t="s">
+        <v>612</v>
+      </c>
+      <c r="B77" t="s">
+        <v>868</v>
+      </c>
+      <c r="C77" s="35" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>606</v>
+      </c>
+      <c r="B78" t="s">
+        <v>868</v>
+      </c>
+      <c r="C78" s="35" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>607</v>
+      </c>
+      <c r="B79" t="s">
+        <v>868</v>
+      </c>
+      <c r="C79" s="35" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>613</v>
+      </c>
+      <c r="B80" t="s">
+        <v>868</v>
+      </c>
+      <c r="C80" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>614</v>
+      </c>
+      <c r="B81" t="s">
+        <v>868</v>
+      </c>
+      <c r="C81" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>616</v>
+      </c>
+      <c r="B82" t="s">
+        <v>868</v>
+      </c>
+      <c r="C82" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>615</v>
+      </c>
+      <c r="B83" t="s">
+        <v>868</v>
+      </c>
+      <c r="C83" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>617</v>
+      </c>
+      <c r="B84" t="s">
+        <v>868</v>
+      </c>
+      <c r="C84" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>618</v>
+      </c>
+      <c r="B85" t="s">
+        <v>868</v>
+      </c>
+      <c r="C85" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>619</v>
+      </c>
+      <c r="B86" t="s">
+        <v>868</v>
+      </c>
+      <c r="C86" s="35" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>620</v>
+      </c>
+      <c r="B87" t="s">
+        <v>868</v>
+      </c>
+      <c r="C87" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>621</v>
+      </c>
+      <c r="B88" t="s">
+        <v>868</v>
+      </c>
+      <c r="C88" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>622</v>
+      </c>
+      <c r="B89" t="s">
+        <v>868</v>
+      </c>
+      <c r="C89" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>623</v>
+      </c>
+      <c r="B90" t="s">
+        <v>868</v>
+      </c>
+      <c r="C90" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>624</v>
+      </c>
+      <c r="B91" t="s">
+        <v>868</v>
+      </c>
+      <c r="C91" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>625</v>
+      </c>
+      <c r="B92" t="s">
+        <v>868</v>
+      </c>
+      <c r="C92" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>626</v>
+      </c>
+      <c r="B93" t="s">
+        <v>868</v>
+      </c>
+      <c r="C93" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>627</v>
+      </c>
+      <c r="B94" t="s">
+        <v>868</v>
+      </c>
+      <c r="C94" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>628</v>
+      </c>
+      <c r="B95" t="s">
+        <v>868</v>
+      </c>
+      <c r="C95" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>629</v>
+      </c>
+      <c r="B96" t="s">
+        <v>868</v>
+      </c>
+      <c r="C96" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>630</v>
+      </c>
+      <c r="B97" t="s">
+        <v>868</v>
+      </c>
+      <c r="C97" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>631</v>
+      </c>
+      <c r="B98" t="s">
+        <v>868</v>
+      </c>
+      <c r="C98" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>632</v>
+      </c>
+      <c r="B99" t="s">
+        <v>868</v>
+      </c>
+      <c r="C99" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>633</v>
+      </c>
+      <c r="B100" t="s">
+        <v>868</v>
+      </c>
+      <c r="C100" s="35" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>737</v>
+      </c>
+      <c r="B101" t="s">
+        <v>868</v>
+      </c>
+      <c r="C101" s="35" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>738</v>
+      </c>
+      <c r="B102" t="s">
+        <v>868</v>
+      </c>
+      <c r="C102" s="35" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>640</v>
+      </c>
+      <c r="B103" t="s">
+        <v>868</v>
+      </c>
+      <c r="C103" s="35" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>641</v>
+      </c>
+      <c r="B104" t="s">
+        <v>868</v>
+      </c>
+      <c r="C104" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>642</v>
+      </c>
+      <c r="B105" t="s">
+        <v>868</v>
+      </c>
+      <c r="C105" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>643</v>
+      </c>
+      <c r="B106" t="s">
+        <v>868</v>
+      </c>
+      <c r="C106" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>644</v>
+      </c>
+      <c r="B107" t="s">
+        <v>868</v>
+      </c>
+      <c r="C107" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>645</v>
+      </c>
+      <c r="B108" t="s">
+        <v>868</v>
+      </c>
+      <c r="C108" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>646</v>
+      </c>
+      <c r="B109" t="s">
+        <v>868</v>
+      </c>
+      <c r="C109" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>647</v>
+      </c>
+      <c r="B110" t="s">
+        <v>868</v>
+      </c>
+      <c r="C110" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>648</v>
+      </c>
+      <c r="B111" t="s">
+        <v>868</v>
+      </c>
+      <c r="C111" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>649</v>
+      </c>
+      <c r="B112" t="s">
+        <v>868</v>
+      </c>
+      <c r="C112" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>650</v>
+      </c>
+      <c r="B113" t="s">
+        <v>868</v>
+      </c>
+      <c r="C113" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>651</v>
+      </c>
+      <c r="B114" t="s">
+        <v>868</v>
+      </c>
+      <c r="C114" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>652</v>
+      </c>
+      <c r="B115" t="s">
+        <v>868</v>
+      </c>
+      <c r="C115" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>653</v>
+      </c>
+      <c r="B116" t="s">
+        <v>868</v>
+      </c>
+      <c r="C116" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>654</v>
+      </c>
+      <c r="B117" t="s">
+        <v>868</v>
+      </c>
+      <c r="C117" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>655</v>
+      </c>
+      <c r="B118" t="s">
+        <v>868</v>
+      </c>
+      <c r="C118" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>656</v>
+      </c>
+      <c r="B119" t="s">
+        <v>868</v>
+      </c>
+      <c r="C119" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>657</v>
+      </c>
+      <c r="B120" t="s">
+        <v>868</v>
+      </c>
+      <c r="C120" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>658</v>
+      </c>
+      <c r="B121" t="s">
+        <v>868</v>
+      </c>
+      <c r="C121" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>659</v>
+      </c>
+      <c r="B122" t="s">
+        <v>868</v>
+      </c>
+      <c r="C122" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>660</v>
+      </c>
+      <c r="B123" t="s">
+        <v>868</v>
+      </c>
+      <c r="C123" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>661</v>
+      </c>
+      <c r="B124" t="s">
+        <v>868</v>
+      </c>
+      <c r="C124" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>662</v>
+      </c>
+      <c r="B125" t="s">
+        <v>868</v>
+      </c>
+      <c r="C125" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>663</v>
+      </c>
+      <c r="B126" t="s">
+        <v>868</v>
+      </c>
+      <c r="C126" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>664</v>
+      </c>
+      <c r="B127" t="s">
+        <v>868</v>
+      </c>
+      <c r="C127" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>665</v>
+      </c>
+      <c r="B128" t="s">
+        <v>868</v>
+      </c>
+      <c r="C128" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>666</v>
+      </c>
+      <c r="B129" t="s">
+        <v>868</v>
+      </c>
+      <c r="C129" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>667</v>
+      </c>
+      <c r="B130" t="s">
+        <v>868</v>
+      </c>
+      <c r="C130" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>668</v>
+      </c>
+      <c r="B131" t="s">
+        <v>868</v>
+      </c>
+      <c r="C131" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>669</v>
+      </c>
+      <c r="B132" t="s">
+        <v>868</v>
+      </c>
+      <c r="C132" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>670</v>
+      </c>
+      <c r="B133" t="s">
+        <v>868</v>
+      </c>
+      <c r="C133" s="35" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>671</v>
+      </c>
+      <c r="B134" t="s">
+        <v>868</v>
+      </c>
+      <c r="C134" s="35" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>672</v>
+      </c>
+      <c r="B135" t="s">
+        <v>868</v>
+      </c>
+      <c r="C135" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>673</v>
+      </c>
+      <c r="B136" t="s">
+        <v>868</v>
+      </c>
+      <c r="C136" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>674</v>
+      </c>
+      <c r="B137" t="s">
+        <v>868</v>
+      </c>
+      <c r="C137" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>675</v>
+      </c>
+      <c r="B138" t="s">
+        <v>868</v>
+      </c>
+      <c r="C138" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>676</v>
+      </c>
+      <c r="B139" t="s">
+        <v>868</v>
+      </c>
+      <c r="C139" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>677</v>
+      </c>
+      <c r="B140" t="s">
+        <v>868</v>
+      </c>
+      <c r="C140" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>678</v>
+      </c>
+      <c r="B141" t="s">
+        <v>868</v>
+      </c>
+      <c r="C141" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>679</v>
+      </c>
+      <c r="B142" t="s">
+        <v>868</v>
+      </c>
+      <c r="C142" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>680</v>
+      </c>
+      <c r="B143" t="s">
+        <v>868</v>
+      </c>
+      <c r="C143" s="35" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>681</v>
+      </c>
+      <c r="B144" t="s">
+        <v>868</v>
+      </c>
+      <c r="C144" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>682</v>
+      </c>
+      <c r="B145" t="s">
+        <v>868</v>
+      </c>
+      <c r="C145" s="35" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>683</v>
+      </c>
+      <c r="B146" t="s">
+        <v>868</v>
+      </c>
+      <c r="C146" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>684</v>
+      </c>
+      <c r="B147" t="s">
+        <v>868</v>
+      </c>
+      <c r="C147" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>685</v>
+      </c>
+      <c r="B148" t="s">
+        <v>868</v>
+      </c>
+      <c r="C148" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>686</v>
+      </c>
+      <c r="B149" t="s">
+        <v>868</v>
+      </c>
+      <c r="C149" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>687</v>
+      </c>
+      <c r="B150" t="s">
+        <v>868</v>
+      </c>
+      <c r="C150" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>688</v>
+      </c>
+      <c r="B151" t="s">
+        <v>868</v>
+      </c>
+      <c r="C151" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>689</v>
+      </c>
+      <c r="B152" t="s">
+        <v>868</v>
+      </c>
+      <c r="C152" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>690</v>
+      </c>
+      <c r="B153" t="s">
+        <v>868</v>
+      </c>
+      <c r="C153" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>691</v>
+      </c>
+      <c r="B154" t="s">
+        <v>868</v>
+      </c>
+      <c r="C154" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>692</v>
+      </c>
+      <c r="B155" t="s">
+        <v>868</v>
+      </c>
+      <c r="C155" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>693</v>
+      </c>
+      <c r="B156" t="s">
+        <v>868</v>
+      </c>
+      <c r="C156" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>694</v>
+      </c>
+      <c r="B157" t="s">
+        <v>868</v>
+      </c>
+      <c r="C157" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>695</v>
+      </c>
+      <c r="B158" t="s">
+        <v>868</v>
+      </c>
+      <c r="C158" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>696</v>
+      </c>
+      <c r="B159" t="s">
+        <v>868</v>
+      </c>
+      <c r="C159" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>697</v>
+      </c>
+      <c r="B160" t="s">
+        <v>868</v>
+      </c>
+      <c r="C160" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>698</v>
+      </c>
+      <c r="B161" t="s">
+        <v>868</v>
+      </c>
+      <c r="C161" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>699</v>
+      </c>
+      <c r="B162" t="s">
+        <v>868</v>
+      </c>
+      <c r="C162" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>700</v>
+      </c>
+      <c r="B163" t="s">
+        <v>868</v>
+      </c>
+      <c r="C163" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>701</v>
+      </c>
+      <c r="B164" t="s">
+        <v>868</v>
+      </c>
+      <c r="C164" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>702</v>
+      </c>
+      <c r="B165" t="s">
+        <v>868</v>
+      </c>
+      <c r="C165" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>703</v>
+      </c>
+      <c r="B166" t="s">
+        <v>868</v>
+      </c>
+      <c r="C166" s="35" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>704</v>
+      </c>
+      <c r="B167" t="s">
+        <v>868</v>
+      </c>
+      <c r="C167" s="35" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>705</v>
+      </c>
+      <c r="B168" t="s">
+        <v>868</v>
+      </c>
+      <c r="C168" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>706</v>
+      </c>
+      <c r="B169" t="s">
+        <v>868</v>
+      </c>
+      <c r="C169" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
+        <v>707</v>
+      </c>
+      <c r="B170" t="s">
+        <v>868</v>
+      </c>
+      <c r="C170" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>708</v>
+      </c>
+      <c r="B171" t="s">
+        <v>868</v>
+      </c>
+      <c r="C171" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>709</v>
+      </c>
+      <c r="B172" t="s">
+        <v>868</v>
+      </c>
+      <c r="C172" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>710</v>
+      </c>
+      <c r="B173" t="s">
+        <v>868</v>
+      </c>
+      <c r="C173" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>711</v>
+      </c>
+      <c r="B174" t="s">
+        <v>868</v>
+      </c>
+      <c r="C174" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
+        <v>712</v>
+      </c>
+      <c r="B175" t="s">
+        <v>868</v>
+      </c>
+      <c r="C175" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
+        <v>713</v>
+      </c>
+      <c r="B176" t="s">
+        <v>868</v>
+      </c>
+      <c r="C176" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" t="s">
+        <v>714</v>
+      </c>
+      <c r="B177" t="s">
+        <v>868</v>
+      </c>
+      <c r="C177" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" t="s">
+        <v>715</v>
+      </c>
+      <c r="B178" t="s">
+        <v>868</v>
+      </c>
+      <c r="C178" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>716</v>
+      </c>
+      <c r="B179" t="s">
+        <v>868</v>
+      </c>
+      <c r="C179" s="35" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" t="s">
+        <v>634</v>
+      </c>
+      <c r="B180" t="s">
+        <v>868</v>
+      </c>
+      <c r="C180" s="35" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" t="s">
+        <v>717</v>
+      </c>
+      <c r="B181" t="s">
+        <v>868</v>
+      </c>
+      <c r="C181" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
+        <v>718</v>
+      </c>
+      <c r="B182" t="s">
+        <v>868</v>
+      </c>
+      <c r="C182" s="35" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>778</v>
+      </c>
+      <c r="B183" t="s">
+        <v>868</v>
+      </c>
+      <c r="C183" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
+        <v>779</v>
+      </c>
+      <c r="B184" t="s">
+        <v>868</v>
+      </c>
+      <c r="C184" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" t="s">
+        <v>781</v>
+      </c>
+      <c r="B185" t="s">
+        <v>868</v>
+      </c>
+      <c r="C185" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>782</v>
+      </c>
+      <c r="B186" t="s">
+        <v>868</v>
+      </c>
+      <c r="C186" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>783</v>
+      </c>
+      <c r="B187" t="s">
+        <v>868</v>
+      </c>
+      <c r="C187" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>784</v>
+      </c>
+      <c r="B188" t="s">
+        <v>868</v>
+      </c>
+      <c r="C188" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" t="s">
+        <v>785</v>
+      </c>
+      <c r="B189" t="s">
+        <v>868</v>
+      </c>
+      <c r="C189" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>786</v>
+      </c>
+      <c r="B190" t="s">
+        <v>868</v>
+      </c>
+      <c r="C190" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" t="s">
+        <v>787</v>
+      </c>
+      <c r="B191" t="s">
+        <v>868</v>
+      </c>
+      <c r="C191" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
+        <v>788</v>
+      </c>
+      <c r="B192" t="s">
+        <v>868</v>
+      </c>
+      <c r="C192" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
+        <v>789</v>
+      </c>
+      <c r="B193" t="s">
+        <v>868</v>
+      </c>
+      <c r="C193" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" t="s">
+        <v>790</v>
+      </c>
+      <c r="B194" t="s">
+        <v>868</v>
+      </c>
+      <c r="C194" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" t="s">
+        <v>791</v>
+      </c>
+      <c r="B195" t="s">
+        <v>868</v>
+      </c>
+      <c r="C195" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" t="s">
+        <v>792</v>
+      </c>
+      <c r="B196" t="s">
+        <v>868</v>
+      </c>
+      <c r="C196" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
+        <v>793</v>
+      </c>
+      <c r="B197" t="s">
+        <v>868</v>
+      </c>
+      <c r="C197" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
+        <v>794</v>
+      </c>
+      <c r="B198" t="s">
+        <v>868</v>
+      </c>
+      <c r="C198" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>795</v>
+      </c>
+      <c r="B199" t="s">
+        <v>868</v>
+      </c>
+      <c r="C199" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
+        <v>796</v>
+      </c>
+      <c r="B200" t="s">
+        <v>868</v>
+      </c>
+      <c r="C200" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>797</v>
+      </c>
+      <c r="B201" t="s">
+        <v>868</v>
+      </c>
+      <c r="C201" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" t="s">
+        <v>798</v>
+      </c>
+      <c r="B202" t="s">
+        <v>868</v>
+      </c>
+      <c r="C202" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>799</v>
+      </c>
+      <c r="B203" t="s">
+        <v>868</v>
+      </c>
+      <c r="C203" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
+        <v>800</v>
+      </c>
+      <c r="B204" t="s">
+        <v>868</v>
+      </c>
+      <c r="C204" s="35" t="s">
+        <v>830</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A71:A177">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A71:A204">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -15837,10 +18490,10 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -15888,7 +18541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -15896,7 +18549,7 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -16042,23 +18695,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="12.75" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
@@ -16246,12 +18899,12 @@
       <selection activeCell="D3" sqref="D3:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="24.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16259,12 +18912,12 @@
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>721</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -16382,9 +19035,9 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16392,12 +19045,12 @@
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -16563,23 +19216,23 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.75" customWidth="1"/>
-    <col min="3" max="3" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -16709,24 +19362,24 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -17033,23 +19686,23 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -17170,10 +19823,10 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08203125" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17181,12 +19834,12 @@
       <c r="A1" s="19" t="s">
         <v>396</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -17777,6 +20430,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -18029,7 +20690,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -18038,15 +20699,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18065,27 +20735,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating with changed Sierra Leone villages
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sparrowdscom-my.sharepoint.com/personal/kevin_sparrowds_com/Documents/GIS Data/TBM/TBM Github/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFD9D0D-424B-47D9-8BBF-209481FFF540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{FEFD9D0D-424B-47D9-8BBF-209481FFF540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3443726-DDC0-40DF-A568-B5782A677AD2}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15571" tabRatio="813" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27727" yWindow="14305" windowWidth="28012" windowHeight="14413" tabRatio="813" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -18,48 +18,50 @@
     <sheet name="TBMAR" sheetId="9" r:id="rId3"/>
     <sheet name="TBMBS" sheetId="36" r:id="rId4"/>
     <sheet name="TBMBW" sheetId="39" r:id="rId5"/>
-    <sheet name="TBMCV" sheetId="15" r:id="rId6"/>
-    <sheet name="TBMFI" sheetId="24" r:id="rId7"/>
-    <sheet name="TBMG" sheetId="26" r:id="rId8"/>
-    <sheet name="TBMI" sheetId="27" r:id="rId9"/>
-    <sheet name="TBMNJ" sheetId="11" r:id="rId10"/>
-    <sheet name="TBMKA" sheetId="5" r:id="rId11"/>
-    <sheet name="TBMK" sheetId="4" r:id="rId12"/>
-    <sheet name="TBMKI" sheetId="10" r:id="rId13"/>
-    <sheet name="TBMKS" sheetId="35" r:id="rId14"/>
-    <sheet name="TBMM" sheetId="23" r:id="rId15"/>
-    <sheet name="TBMN" sheetId="28" r:id="rId16"/>
-    <sheet name="TBMNG" sheetId="29" r:id="rId17"/>
-    <sheet name="TBMGN" sheetId="6" r:id="rId18"/>
-    <sheet name="TBMGT" sheetId="32" r:id="rId19"/>
-    <sheet name="TBMQ" sheetId="25" r:id="rId20"/>
-    <sheet name="TBMSA" sheetId="31" r:id="rId21"/>
-    <sheet name="Go_Build_Love" sheetId="17" r:id="rId22"/>
-    <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId23"/>
-    <sheet name="Serve_Hope" sheetId="21" r:id="rId24"/>
-    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId25"/>
-    <sheet name="Wifi_Materials" sheetId="37" r:id="rId26"/>
-    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId27"/>
-    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId28"/>
-    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId29"/>
+    <sheet name="TBMPB" sheetId="41" r:id="rId6"/>
+    <sheet name="TBMCV" sheetId="15" r:id="rId7"/>
+    <sheet name="TBMFI" sheetId="24" r:id="rId8"/>
+    <sheet name="TBMG" sheetId="26" r:id="rId9"/>
+    <sheet name="TBMI" sheetId="27" r:id="rId10"/>
+    <sheet name="TBMNJ" sheetId="11" r:id="rId11"/>
+    <sheet name="TBMKA" sheetId="5" r:id="rId12"/>
+    <sheet name="TBMK" sheetId="4" r:id="rId13"/>
+    <sheet name="TBMKI" sheetId="10" r:id="rId14"/>
+    <sheet name="TBMKS" sheetId="35" r:id="rId15"/>
+    <sheet name="TBMM" sheetId="23" r:id="rId16"/>
+    <sheet name="TBMN" sheetId="28" r:id="rId17"/>
+    <sheet name="TBMNG" sheetId="29" r:id="rId18"/>
+    <sheet name="TBMGN" sheetId="6" r:id="rId19"/>
+    <sheet name="TBMGT" sheetId="32" r:id="rId20"/>
+    <sheet name="TBMQ" sheetId="25" r:id="rId21"/>
+    <sheet name="TBMSA" sheetId="31" r:id="rId22"/>
+    <sheet name="TBMSL" sheetId="40" r:id="rId23"/>
+    <sheet name="Go_Build_Love" sheetId="17" r:id="rId24"/>
+    <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId25"/>
+    <sheet name="Serve_Hope" sheetId="21" r:id="rId26"/>
+    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId27"/>
+    <sheet name="Wifi_Materials" sheetId="37" r:id="rId28"/>
+    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId29"/>
+    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId30"/>
+    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId31"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId30"/>
+    <externalReference r:id="rId32"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
-    <definedName name="Reserved" localSheetId="21">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="22">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
     <definedName name="Reserved" localSheetId="23">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="24">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="25">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="0">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="1">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="2">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="5">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="7">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="17">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="6">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="8">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="18">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="11">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="13">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="10">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="12">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="9">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Special">[1]types!$A$169:$A$177</definedName>
   </definedNames>
@@ -80,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4255" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="975">
   <si>
     <t>Latitude</t>
   </si>
@@ -2847,19 +2849,206 @@
   </si>
   <si>
     <t>WaiWai</t>
+  </si>
+  <si>
+    <t>The Bucket Ministry Sierra Leone</t>
+  </si>
+  <si>
+    <t>Krio</t>
+  </si>
+  <si>
+    <t>Themne</t>
+  </si>
+  <si>
+    <t>Mende</t>
+  </si>
+  <si>
+    <t>Fullah</t>
+  </si>
+  <si>
+    <t>Geeta Nagar</t>
+  </si>
+  <si>
+    <t>Oloisinyai A</t>
+  </si>
+  <si>
+    <t>Oloiisinyai B</t>
+  </si>
+  <si>
+    <t>Eremit</t>
+  </si>
+  <si>
+    <t>Kikuro</t>
+  </si>
+  <si>
+    <t>Emilango</t>
+  </si>
+  <si>
+    <t>Embash</t>
+  </si>
+  <si>
+    <t>Lesokoro</t>
+  </si>
+  <si>
+    <t>Intinyika</t>
+  </si>
+  <si>
+    <t>Nolesencha</t>
+  </si>
+  <si>
+    <t>Enkirimbei</t>
+  </si>
+  <si>
+    <t>Inkeek otoito</t>
+  </si>
+  <si>
+    <t>Enkare kiti</t>
+  </si>
+  <si>
+    <t>Kisidai</t>
+  </si>
+  <si>
+    <t>Newton - Five Mile</t>
+  </si>
+  <si>
+    <t>Newton - Six Mile</t>
+  </si>
+  <si>
+    <t>Newton - Mabanamaton</t>
+  </si>
+  <si>
+    <t>Newton - Crossing</t>
+  </si>
+  <si>
+    <t>Newton - Makoko</t>
+  </si>
+  <si>
+    <t>The Bucket Ministry Besigan</t>
+  </si>
+  <si>
+    <t>Besigan - Centro - 1</t>
+  </si>
+  <si>
+    <t>Besigan - Centro - 2</t>
+  </si>
+  <si>
+    <t>Besigan - Centro - 3</t>
+  </si>
+  <si>
+    <t>Besigan - Centro - 4</t>
+  </si>
+  <si>
+    <t>Besigan - Mahabwa</t>
+  </si>
+  <si>
+    <t>Besigan - Kibanog</t>
+  </si>
+  <si>
+    <t>Besigan - Sitio KM17</t>
+  </si>
+  <si>
+    <t>Besigan - Sitio KM16</t>
+  </si>
+  <si>
+    <t>Besigan - Sitio KM18</t>
+  </si>
+  <si>
+    <t>Besigan - Sitio Kadayonan</t>
+  </si>
+  <si>
+    <t>Besigan - Sitio KM11</t>
+  </si>
+  <si>
+    <t>Besigan - Sitio Kamang</t>
+  </si>
+  <si>
+    <t>Higaonon</t>
+  </si>
+  <si>
+    <t>Muslim</t>
+  </si>
+  <si>
+    <t>Bisaya</t>
+  </si>
+  <si>
+    <t>Ilonggo</t>
+  </si>
+  <si>
+    <t>llonggo</t>
+  </si>
+  <si>
+    <t>Tagalog</t>
+  </si>
+  <si>
+    <t>Grafton - PVA/Joshua</t>
+  </si>
+  <si>
+    <t>Grafton - Forut</t>
+  </si>
+  <si>
+    <t>Grafton - Cyprus</t>
+  </si>
+  <si>
+    <t>Grafton - Town</t>
+  </si>
+  <si>
+    <t>Grafton - New camp</t>
+  </si>
+  <si>
+    <t>Grafton - Barracks</t>
+  </si>
+  <si>
+    <t>Grafton - Old camp</t>
+  </si>
+  <si>
+    <t>Grafton - SOJA town</t>
+  </si>
+  <si>
+    <t>Grafton - CRS</t>
+  </si>
+  <si>
+    <t>Grafton - Scout camp area</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="30">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3031,6 +3220,12 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3061,77 +3256,97 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3142,11 +3357,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="14">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{7EFD0C81-D916-49C9-94DE-10796A385AC6}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{C6976ACF-4CF3-445D-A0DA-B78AF634B62B}"/>
     <cellStyle name="Normal 3 2" xfId="3" xr:uid="{7CE6C237-AEFB-4568-BA38-55AF6AE605BA}"/>
+    <cellStyle name="Normal 3 2 2" xfId="5" xr:uid="{90F56A41-647C-4C34-BD45-B54BB107D25B}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="11" xr:uid="{F287E36A-8B60-4482-9D1A-890E141B5C84}"/>
+    <cellStyle name="Normal 3 2 3" xfId="7" xr:uid="{A15A4427-7995-4B5D-A1D7-F367306A1B75}"/>
+    <cellStyle name="Normal 3 2 3 2" xfId="13" xr:uid="{9010AFFF-EC58-4437-ACA5-04B7668B19BE}"/>
+    <cellStyle name="Normal 3 2 4" xfId="9" xr:uid="{8A3695EE-AB81-445F-B8EE-3E6A03BA18FD}"/>
+    <cellStyle name="Normal 3 3" xfId="4" xr:uid="{1DF893BE-2ACB-4919-A7CD-AA2C21148360}"/>
+    <cellStyle name="Normal 3 3 2" xfId="10" xr:uid="{40634298-0337-45B1-B18B-0027A4E75F05}"/>
+    <cellStyle name="Normal 3 4" xfId="6" xr:uid="{1D4019B0-C20C-4A7E-97DB-AC8FFD25DB45}"/>
+    <cellStyle name="Normal 3 4 2" xfId="12" xr:uid="{3DEC3C28-17B5-4A3F-91B5-B6EF8513FB54}"/>
+    <cellStyle name="Normal 3 5" xfId="8" xr:uid="{50844260-08FF-46B0-B10D-4A4539C5FF24}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -3593,24 +3818,24 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
@@ -3764,6 +3989,143 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928B598D-2E02-41AD-A7FC-B205F15DB675}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" s="6" t="s">
+        <v>283</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{276EC5A8-C0AD-4544-963F-0C6C26A08E3E}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4914AC-81CB-46C7-BD71-CF158ABA186A}">
   <dimension ref="A1:E78"/>
   <sheetViews>
@@ -3771,23 +4133,23 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.125" customWidth="1"/>
-    <col min="3" max="3" width="9.3125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -4377,7 +4739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5B793A-E672-42F0-B7CD-796F921CC77D}">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -4385,23 +4747,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
@@ -4905,7 +5267,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4922,7 +5284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FCEA8E-D73A-4C32-A54F-932DBA63E3E9}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -4930,23 +5292,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5224,7 +5586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7D1E55-F368-41C4-B6DD-BDC21E354B8B}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -5232,22 +5594,22 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5466,33 +5828,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39F5EFB-4C75-4F45-95CF-B50496BF741C}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A10" sqref="A10:A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>502</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
       <c r="F1" s="19" t="s">
         <v>503</v>
       </c>
@@ -5556,6 +5918,71 @@
     <row r="9" spans="1:7">
       <c r="A9" s="23" t="s">
         <v>585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>940</v>
       </c>
     </row>
   </sheetData>
@@ -5566,7 +5993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7208EC-C09B-46BC-9208-53E975DA3383}">
   <dimension ref="A1:E34"/>
   <sheetViews>
@@ -5574,23 +6001,23 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="24.8125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.8125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>878</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5899,7 +6326,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00598E5C-D8DC-4176-B37C-0365BB6BC78A}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -5907,24 +6334,24 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.8125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6155,7 +6582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14823A46-4501-4F96-80B3-10A0CC5D20D3}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -6163,24 +6590,24 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.8125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6336,7 +6763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E969F7E-8CCE-43F9-9791-7FA2BD394061}">
   <dimension ref="A1:E30"/>
   <sheetViews>
@@ -6344,24 +6771,24 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="41" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6720,131 +7147,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9796B9BC-A579-4EDE-99EB-40D54CC290A0}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>409</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="18"/>
-      <c r="B4" s="3"/>
-      <c r="D4" s="18" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="18"/>
-      <c r="B5" s="3"/>
-      <c r="D5" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="18"/>
-      <c r="B6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="18"/>
-      <c r="B7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8" s="3"/>
-      <c r="D8" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="B9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7447B9F4-0C04-4150-84C1-90BA9C788285}">
-          <x14:formula1>
-            <xm:f>Validation!$B$1:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E4:E1048576 E3</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED93ADC1-EA4D-4904-988A-97AFBF8ADB04}">
   <dimension ref="A1:E27"/>
@@ -6853,23 +7155,23 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7022,6 +7324,131 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9796B9BC-A579-4EDE-99EB-40D54CC290A0}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="18"/>
+      <c r="B4" s="3"/>
+      <c r="D4" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="18"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="18"/>
+      <c r="B6" s="2"/>
+      <c r="D6" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="18"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7447B9F4-0C04-4150-84C1-90BA9C788285}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E1048576 E3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0B993E-AFCD-4B7D-9D40-53D866792064}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7029,24 +7456,24 @@
       <selection activeCell="D3" sqref="D3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7066,7 +7493,7 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>884</v>
       </c>
       <c r="B3" t="s">
@@ -7253,7 +7680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748FCB8D-0FD0-4AE3-B979-7656B5CF254B}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -7261,22 +7688,22 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>408</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7389,7 +7816,182 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>922</v>
+      </c>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="37" t="s">
+        <v>942</v>
+      </c>
+      <c r="C3" t="s">
+        <v>923</v>
+      </c>
+      <c r="D3" t="s">
+        <v>923</v>
+      </c>
+      <c r="E3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="37" t="s">
+        <v>941</v>
+      </c>
+      <c r="C4" t="s">
+        <v>924</v>
+      </c>
+      <c r="D4" t="s">
+        <v>924</v>
+      </c>
+      <c r="E4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="37" t="s">
+        <v>943</v>
+      </c>
+      <c r="C5" t="s">
+        <v>925</v>
+      </c>
+      <c r="D5" t="s">
+        <v>925</v>
+      </c>
+      <c r="E5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="37" t="s">
+        <v>944</v>
+      </c>
+      <c r="C6" t="s">
+        <v>926</v>
+      </c>
+      <c r="D6" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="37" t="s">
+        <v>945</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="42" t="s">
+        <v>965</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="42" t="s">
+        <v>966</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="42" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="42" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="42" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="42" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="42" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="42" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="42" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="42" t="s">
+        <v>974</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD20C374-E3CD-408E-8EB0-BA328822C0D2}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E24D227-6B92-4869-A6EE-2CD0CE718ADB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7397,23 +7999,23 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7565,7 +8167,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E0DFFC-07E8-40BE-8CA3-81702524BE9F}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7573,22 +8175,22 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>407</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7740,7 +8342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8966E3F0-5F1C-45DE-88BD-0792C7795602}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7748,23 +8350,23 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7916,7 +8518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}">
   <dimension ref="A1:D636"/>
   <sheetViews>
@@ -7924,11 +8526,11 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.8125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.8125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -16844,7 +17446,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -16852,11 +17454,11 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.375" customWidth="1"/>
-    <col min="3" max="3" width="59.125" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -16870,7 +17472,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="315">
+    <row r="2" spans="1:3" ht="326.05">
       <c r="A2" t="s">
         <v>811</v>
       </c>
@@ -16936,7 +17538,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="189">
+    <row r="8" spans="1:3" ht="195.65">
       <c r="A8" t="s">
         <v>812</v>
       </c>
@@ -16991,7 +17593,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="252">
+    <row r="13" spans="1:3" ht="260.85000000000002">
       <c r="A13" s="34" t="s">
         <v>830</v>
       </c>
@@ -17007,7 +17609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
   <dimension ref="A1:C204"/>
   <sheetViews>
@@ -17015,10 +17617,10 @@
       <selection activeCell="C2" sqref="C2:C204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="16.3"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="65" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17768,7 +18370,7 @@
     <row r="70" spans="1:3">
       <c r="C70" s="33"/>
     </row>
-    <row r="71" spans="1:3" ht="173.25">
+    <row r="71" spans="1:3" ht="179.35">
       <c r="A71" t="s">
         <v>442</v>
       </c>
@@ -17790,7 +18392,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="47.25">
+    <row r="73" spans="1:3" ht="48.9">
       <c r="A73" t="s">
         <v>604</v>
       </c>
@@ -17801,7 +18403,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="47.25">
+    <row r="74" spans="1:3" ht="48.9">
       <c r="A74" t="s">
         <v>605</v>
       </c>
@@ -17812,7 +18414,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="47.25">
+    <row r="75" spans="1:3" ht="48.9">
       <c r="A75" t="s">
         <v>606</v>
       </c>
@@ -17823,7 +18425,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="47.25">
+    <row r="76" spans="1:3" ht="48.9">
       <c r="A76" t="s">
         <v>607</v>
       </c>
@@ -17834,7 +18436,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="47.25">
+    <row r="77" spans="1:3" ht="48.9">
       <c r="A77" t="s">
         <v>608</v>
       </c>
@@ -19249,211 +19851,6 @@
   <conditionalFormatting sqref="A71:A204">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>417</v>
-      </c>
-      <c r="B1" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>442</v>
-      </c>
-      <c r="B2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>420</v>
-      </c>
-      <c r="B3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>483</v>
-      </c>
-      <c r="B4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B5" t="s">
-        <v>485</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19466,23 +19863,23 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="12.8125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
@@ -19662,6 +20059,211 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>483</v>
+      </c>
+      <c r="B4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B5" t="s">
+        <v>485</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48DAFCB3-68A1-2E4F-90B5-28402B602D58}">
   <dimension ref="A1:E37"/>
@@ -19670,25 +20272,25 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>715</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -19931,7 +20533,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -19952,29 +20554,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53C3151-8CF5-4BEA-BB67-078C4B35658D}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="24.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>900</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -20150,6 +20752,173 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B526CDD-A2A0-4998-84BE-E9C02134A516}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>946</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="38" t="s">
+        <v>947</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>959</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>959</v>
+      </c>
+      <c r="E3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="38" t="s">
+        <v>948</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="39" t="s">
+        <v>960</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>961</v>
+      </c>
+      <c r="E4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="38" t="s">
+        <v>949</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="39" t="s">
+        <v>962</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>963</v>
+      </c>
+      <c r="E5" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="38" t="s">
+        <v>950</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="39" t="s">
+        <v>961</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="38" t="s">
+        <v>951</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="38" t="s">
+        <v>952</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="38" t="s">
+        <v>953</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="38" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="38" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="38" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="38" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="38" t="s">
+        <v>958</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0E8DD59-A49F-4B5C-9C95-FF2EA074B6D6}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C0D976E-CC6E-4E1D-A906-68C6C6E200AE}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -20157,22 +20926,22 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -20330,31 +21099,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95287EDE-9CCE-4714-8045-F1CF58B82ECE}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E1048576"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.8125" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -20419,6 +21188,9 @@
       </c>
     </row>
     <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>927</v>
+      </c>
       <c r="C6" s="6" t="s">
         <v>277</v>
       </c>
@@ -20476,7 +21248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{416149FA-89DB-4D73-B2F5-643855944FF3}">
   <dimension ref="A1:E30"/>
   <sheetViews>
@@ -20484,24 +21256,24 @@
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.3"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="19" t="s">
         <v>393</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="40" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -20789,143 +21561,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FB1E2A62-71F5-4950-8694-49C710CC2DC1}">
-          <x14:formula1>
-            <xm:f>Validation!$B$1:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928B598D-2E02-41AD-A7FC-B205F15DB675}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.8125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>399</v>
-      </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="C4" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="E4" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="C5" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="E5" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="C6" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="C7" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="C8" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9" s="6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="D10" s="6" t="s">
-        <v>283</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{276EC5A8-C0AD-4544-963F-0C6C26A08E3E}">
           <x14:formula1>
             <xm:f>Validation!$B$1:$B$5</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Updating with Shompole Partner Org Changes
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\SparrowGIT\Organization-Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACDB2A9-95BF-451A-AC21-AEE5131A860C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{966CF973-7237-40FD-9576-B7D971DD5AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="813" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="885" windowWidth="25905" windowHeight="15300" tabRatio="813" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4415" uniqueCount="1038">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4432" uniqueCount="1055">
   <si>
     <t>Latitude</t>
   </si>
@@ -3905,12 +3905,6 @@
     <t>Shompole - Orkungu</t>
   </si>
   <si>
-    <t>Inkiramatiani - Inkiramatiani A</t>
-  </si>
-  <si>
-    <t>Inkiramatiani - Inkiramatiani B</t>
-  </si>
-  <si>
     <t>Pakase - Oloisinyai A</t>
   </si>
   <si>
@@ -4026,6 +4020,63 @@
   </si>
   <si>
     <t>The Bucket Ministry Shompole</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Ntigiya A</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Ntigiya B</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Town A</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Town B</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Olkiramatian</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Oloisinyai</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Ilgoso-loonkishu</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Kimelok</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Ilkilang'u</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Enkonyoro A</t>
+  </si>
+  <si>
+    <t>Olkiramatian - Enkonyoro B</t>
+  </si>
+  <si>
+    <t>Oldorko - Oloserian A</t>
+  </si>
+  <si>
+    <t>Oldorko - Oloserian B</t>
+  </si>
+  <si>
+    <t>Oldorko - Komitii A</t>
+  </si>
+  <si>
+    <t>Oldorko - Komitii B</t>
+  </si>
+  <si>
+    <t>Oldorko - Enkutuk-osero A</t>
+  </si>
+  <si>
+    <t>Oldorko - Ndonyio-orkine</t>
+  </si>
+  <si>
+    <t>Oldorko - Olomayiana</t>
+  </si>
+  <si>
+    <t>Oldorko - Enkutuk-osero B</t>
   </si>
 </sst>
 </file>
@@ -4914,11 +4965,11 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -5092,11 +5143,11 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5229,11 +5280,11 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1875" customWidth="1"/>
+    <col min="3" max="3" width="9.3125" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5843,11 +5894,11 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -6384,15 +6435,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FCEA8E-D73A-4C32-A54F-932DBA63E3E9}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6687,13 +6738,13 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6926,19 +6977,19 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39F5EFB-4C75-4F45-95CF-B50496BF741C}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -6946,7 +6997,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="50" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C1" s="50"/>
       <c r="D1" s="50"/>
@@ -7007,12 +7058,12 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="23" t="s">
+      <c r="A8" t="s">
         <v>997</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="23" t="s">
+      <c r="A9" t="s">
         <v>998</v>
       </c>
     </row>
@@ -7132,78 +7183,163 @@
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" t="s">
+      <c r="A33" s="8" t="s">
         <v>1022</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" t="s">
+      <c r="A34" s="8" t="s">
         <v>1023</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="46" t="s">
+      <c r="A35" s="8" t="s">
         <v>1024</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="46" t="s">
+      <c r="A36" s="8" t="s">
         <v>1025</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="8" t="s">
         <v>1026</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="46" t="s">
+      <c r="A38" s="8" t="s">
         <v>1027</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="46" t="s">
+      <c r="A39" s="8" t="s">
         <v>1028</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="46" t="s">
+      <c r="A40" s="8" t="s">
         <v>1029</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="8" t="s">
         <v>1030</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="8" t="s">
         <v>1031</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="8" t="s">
         <v>1032</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="46" t="s">
+      <c r="A44" s="8" t="s">
         <v>1033</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="8" t="s">
         <v>1034</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="46" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="46" t="s">
-        <v>1036</v>
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="46" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="46" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="46" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="46" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="46" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="46" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="46" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="46" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="46" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="46" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="46" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="46" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="46" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="46" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="46" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="46" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="46" t="s">
+        <v>1054</v>
       </c>
     </row>
   </sheetData>
@@ -7222,11 +7358,11 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7555,12 +7691,12 @@
       <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7817,12 +7953,12 @@
       <selection activeCell="E3" sqref="E3:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7998,12 +8134,12 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8382,11 +8518,11 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8558,10 +8694,10 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8683,12 +8819,12 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.4375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8918,12 +9054,12 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.9375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9145,11 +9281,11 @@
       <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9303,10 +9439,10 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9478,11 +9614,11 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9654,10 +9790,10 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9829,11 +9965,11 @@
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10005,11 +10141,11 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -18933,11 +19069,11 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="59.1640625" style="44" customWidth="1"/>
+    <col min="1" max="1" width="24.6875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.3125" customWidth="1"/>
+    <col min="3" max="3" width="59.1875" style="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -18951,7 +19087,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="325.5">
+    <row r="2" spans="1:3" ht="315">
       <c r="A2" t="s">
         <v>800</v>
       </c>
@@ -19017,7 +19153,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="217">
+    <row r="8" spans="1:3" ht="220.5">
       <c r="A8" t="s">
         <v>801</v>
       </c>
@@ -19072,7 +19208,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="248">
+    <row r="13" spans="1:3" ht="236.25">
       <c r="A13" s="34" t="s">
         <v>816</v>
       </c>
@@ -19096,11 +19232,11 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.8125" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -19298,11 +19434,11 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="75.6875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -20051,7 +20187,7 @@
     <row r="70" spans="1:3">
       <c r="C70" s="33"/>
     </row>
-    <row r="71" spans="1:3" ht="170.5">
+    <row r="71" spans="1:3" ht="173.25">
       <c r="A71" t="s">
         <v>439</v>
       </c>
@@ -20073,7 +20209,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="62">
+    <row r="73" spans="1:3" ht="47.25">
       <c r="A73" t="s">
         <v>593</v>
       </c>
@@ -20084,7 +20220,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="62">
+    <row r="74" spans="1:3" ht="47.25">
       <c r="A74" t="s">
         <v>594</v>
       </c>
@@ -20095,7 +20231,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="62">
+    <row r="75" spans="1:3" ht="47.25">
       <c r="A75" t="s">
         <v>595</v>
       </c>
@@ -20106,7 +20242,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="62">
+    <row r="76" spans="1:3" ht="47.25">
       <c r="A76" t="s">
         <v>596</v>
       </c>
@@ -20117,7 +20253,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="62">
+    <row r="77" spans="1:3" ht="47.25">
       <c r="A77" t="s">
         <v>597</v>
       </c>
@@ -20216,7 +20352,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="31">
+    <row r="86" spans="1:3" ht="31.5">
       <c r="A86" t="s">
         <v>604</v>
       </c>
@@ -20238,7 +20374,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="31">
+    <row r="88" spans="1:3" ht="31.5">
       <c r="A88" t="s">
         <v>606</v>
       </c>
@@ -20249,7 +20385,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="31">
+    <row r="89" spans="1:3" ht="31.5">
       <c r="A89" t="s">
         <v>607</v>
       </c>
@@ -20260,7 +20396,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="31">
+    <row r="90" spans="1:3" ht="31.5">
       <c r="A90" t="s">
         <v>608</v>
       </c>
@@ -20271,7 +20407,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="31">
+    <row r="91" spans="1:3" ht="31.5">
       <c r="A91" t="s">
         <v>609</v>
       </c>
@@ -20282,7 +20418,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="31">
+    <row r="92" spans="1:3" ht="31.5">
       <c r="A92" t="s">
         <v>610</v>
       </c>
@@ -20293,7 +20429,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="31">
+    <row r="93" spans="1:3" ht="31.5">
       <c r="A93" t="s">
         <v>611</v>
       </c>
@@ -20304,7 +20440,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="31">
+    <row r="94" spans="1:3" ht="31.5">
       <c r="A94" t="s">
         <v>612</v>
       </c>
@@ -20315,7 +20451,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="31">
+    <row r="95" spans="1:3" ht="31.5">
       <c r="A95" t="s">
         <v>613</v>
       </c>
@@ -20326,7 +20462,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="31">
+    <row r="96" spans="1:3" ht="31.5">
       <c r="A96" t="s">
         <v>614</v>
       </c>
@@ -20337,7 +20473,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="31">
+    <row r="97" spans="1:3" ht="31.5">
       <c r="A97" t="s">
         <v>615</v>
       </c>
@@ -20348,7 +20484,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="31">
+    <row r="98" spans="1:3" ht="31.5">
       <c r="A98" t="s">
         <v>616</v>
       </c>
@@ -20359,7 +20495,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="31">
+    <row r="99" spans="1:3" ht="31.5">
       <c r="A99" t="s">
         <v>617</v>
       </c>
@@ -20370,7 +20506,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="31">
+    <row r="100" spans="1:3" ht="31.5">
       <c r="A100" t="s">
         <v>618</v>
       </c>
@@ -21613,10 +21749,10 @@
       <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -21672,7 +21808,7 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -21818,13 +21954,13 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22104,13 +22240,13 @@
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.3125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22305,10 +22441,10 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22472,10 +22608,10 @@
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22653,11 +22789,11 @@
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.8125" customWidth="1"/>
+    <col min="3" max="3" width="16.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22802,12 +22938,12 @@
       <selection activeCell="E3" sqref="E3:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -23119,20 +23255,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23389,6 +23525,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -23401,14 +23545,6 @@
     <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Updating to add Nyalenda Project
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\SparrowGIT\Organization-Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SparrowGIT\Organization-Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{966CF973-7237-40FD-9576-B7D971DD5AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{81C468A7-275E-40E4-8504-C8DB25068B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="885" windowWidth="25905" windowHeight="15300" tabRatio="813" firstSheet="5" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15511" tabRatio="813" firstSheet="5" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -28,38 +28,39 @@
     <sheet name="TBMK" sheetId="4" r:id="rId13"/>
     <sheet name="TBMKI" sheetId="10" r:id="rId14"/>
     <sheet name="TBMKS" sheetId="35" r:id="rId15"/>
-    <sheet name="TBMM" sheetId="23" r:id="rId16"/>
-    <sheet name="TBMN" sheetId="28" r:id="rId17"/>
-    <sheet name="TBMNG" sheetId="29" r:id="rId18"/>
-    <sheet name="TBMGN" sheetId="6" r:id="rId19"/>
-    <sheet name="TBMGT" sheetId="32" r:id="rId20"/>
-    <sheet name="TBMQN" sheetId="42" r:id="rId21"/>
-    <sheet name="TBMQS" sheetId="25" r:id="rId22"/>
-    <sheet name="TBMSA" sheetId="31" r:id="rId23"/>
-    <sheet name="TBMSL" sheetId="40" r:id="rId24"/>
-    <sheet name="Go_Build_Love" sheetId="17" r:id="rId25"/>
-    <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId26"/>
-    <sheet name="Serve_Hope" sheetId="21" r:id="rId27"/>
-    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId28"/>
-    <sheet name="Wifi_Materials" sheetId="37" r:id="rId29"/>
-    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId30"/>
-    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId31"/>
-    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId32"/>
+    <sheet name="TBMKN" sheetId="43" r:id="rId16"/>
+    <sheet name="TBMM" sheetId="23" r:id="rId17"/>
+    <sheet name="TBMN" sheetId="28" r:id="rId18"/>
+    <sheet name="TBMNG" sheetId="29" r:id="rId19"/>
+    <sheet name="TBMGN" sheetId="6" r:id="rId20"/>
+    <sheet name="TBMGT" sheetId="32" r:id="rId21"/>
+    <sheet name="TBMQN" sheetId="42" r:id="rId22"/>
+    <sheet name="TBMQS" sheetId="25" r:id="rId23"/>
+    <sheet name="TBMSA" sheetId="31" r:id="rId24"/>
+    <sheet name="TBMSL" sheetId="40" r:id="rId25"/>
+    <sheet name="Go_Build_Love" sheetId="17" r:id="rId26"/>
+    <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId27"/>
+    <sheet name="Serve_Hope" sheetId="21" r:id="rId28"/>
+    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId29"/>
+    <sheet name="Wifi_Materials" sheetId="37" r:id="rId30"/>
+    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId31"/>
+    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId32"/>
+    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId33"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId33"/>
+    <externalReference r:id="rId34"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
-    <definedName name="Reserved" localSheetId="24">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="28" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
     <definedName name="Reserved" localSheetId="25">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="26">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="27">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="0">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="1">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="2">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="6">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="8">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="18">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="19">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="11">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="13">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="10">[1]!tblReserved[Reserved keywords]</definedName>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4432" uniqueCount="1055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4473" uniqueCount="1071">
   <si>
     <t>Latitude</t>
   </si>
@@ -4077,6 +4078,54 @@
   </si>
   <si>
     <t>Oldorko - Enkutuk-osero B</t>
+  </si>
+  <si>
+    <t>The Bucket Ministry Nyalenda</t>
+  </si>
+  <si>
+    <t>Nyalenda A - Dago</t>
+  </si>
+  <si>
+    <t>Luos</t>
+  </si>
+  <si>
+    <t>Dholuo</t>
+  </si>
+  <si>
+    <t>Nyalenda A - Kanyakwar</t>
+  </si>
+  <si>
+    <t>Nyalenda A - Kowino</t>
+  </si>
+  <si>
+    <t>Luhyas</t>
+  </si>
+  <si>
+    <t>Ekigusii</t>
+  </si>
+  <si>
+    <t>Nyalenda A - Western A</t>
+  </si>
+  <si>
+    <t>Nyalenda B - Western B</t>
+  </si>
+  <si>
+    <t>Nyalenda B – Kilo</t>
+  </si>
+  <si>
+    <t>Nyalenda B – Kapuothe</t>
+  </si>
+  <si>
+    <t>Nyalenda B - Got Owak</t>
+  </si>
+  <si>
+    <t>Nyalenda B – Nanga</t>
+  </si>
+  <si>
+    <t>Nyalenda B - Dunga</t>
+  </si>
+  <si>
+    <t>Nyalenda A – Capital/Cental</t>
   </si>
 </sst>
 </file>
@@ -4382,7 +4431,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4483,6 +4532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6979,7 +7029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39F5EFB-4C75-4F45-95CF-B50496BF741C}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
@@ -7351,6 +7401,196 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72036BD-30F9-4694-8C78-9BF67137CB5D}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="24.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.4375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="19" t="s">
+        <v>496</v>
+      </c>
+      <c r="G1" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>1059</v>
+      </c>
+      <c r="C4" t="s">
+        <v>501</v>
+      </c>
+      <c r="D4" t="s">
+        <v>343</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C6" t="s">
+        <v>503</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E6" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C8" t="s">
+        <v>470</v>
+      </c>
+      <c r="D8" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D9" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{18C712E4-CE2E-4622-BE04-7D735DBC72E1}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7208EC-C09B-46BC-9208-53E975DA3383}">
   <dimension ref="A1:E34"/>
   <sheetViews>
@@ -7683,7 +7923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00598E5C-D8DC-4176-B37C-0365BB6BC78A}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7945,7 +8185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14823A46-4501-4F96-80B3-10A0CC5D20D3}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -8115,390 +8355,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BA059171-22E3-4BB2-8C57-566D2F497C64}">
-          <x14:formula1>
-            <xm:f>Validation!$B$1:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E969F7E-8CCE-43F9-9791-7FA2BD394061}">
-  <dimension ref="A1:E30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
-        <v>391</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>403</v>
-      </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>441</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>141</v>
-      </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>130</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" t="s">
-        <v>157</v>
-      </c>
-      <c r="D19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" t="s">
-        <v>158</v>
-      </c>
-      <c r="D20" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" t="s">
-        <v>159</v>
-      </c>
-      <c r="D21" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" t="s">
-        <v>160</v>
-      </c>
-      <c r="D22" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="B24" s="3"/>
-      <c r="C24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D24" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="B25" s="3"/>
-      <c r="C25" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="B26" s="3"/>
-      <c r="C26" t="s">
-        <v>164</v>
-      </c>
-      <c r="D26" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="B27" s="3"/>
-      <c r="C27" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="C28" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="C29" t="s">
-        <v>167</v>
-      </c>
-      <c r="D29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="D30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C36A74DD-9932-41E8-8B7D-AE9DB3932DFB}">
           <x14:formula1>
             <xm:f>Validation!$B$1:$B$5</xm:f>
           </x14:formula1>
@@ -8687,6 +8543,390 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E969F7E-8CCE-43F9-9791-7FA2BD394061}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="16.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>403</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>441</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" t="s">
+        <v>153</v>
+      </c>
+      <c r="D15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" s="3"/>
+      <c r="C24" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" s="3"/>
+      <c r="C25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="B26" s="3"/>
+      <c r="C26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="C28" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="C29" t="s">
+        <v>167</v>
+      </c>
+      <c r="D29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="D30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C36A74DD-9932-41E8-8B7D-AE9DB3932DFB}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9796B9BC-A579-4EDE-99EB-40D54CC290A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -8811,7 +9051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E80414F-2A51-4046-8BC5-8F857B02E2CD}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9046,7 +9286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0B993E-AFCD-4B7D-9D40-53D866792064}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9273,7 +9513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748FCB8D-0FD0-4AE3-B979-7656B5CF254B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -9431,7 +9671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -9606,7 +9846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E24D227-6B92-4869-A6EE-2CD0CE718ADB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9782,7 +10022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E0DFFC-07E8-40BE-8CA3-81702524BE9F}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9957,7 +10197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8966E3F0-5F1C-45DE-88BD-0792C7795602}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -10133,7 +10373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}">
   <dimension ref="A1:D636"/>
   <sheetViews>
@@ -19057,169 +19297,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C509">
     <sortCondition ref="A2:A509"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
-  <cols>
-    <col min="1" max="1" width="24.6875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.3125" customWidth="1"/>
-    <col min="3" max="3" width="59.1875" style="44" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>799</v>
-      </c>
-      <c r="B1" t="s">
-        <v>805</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="315">
-      <c r="A2" t="s">
-        <v>800</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>812</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>443</v>
-      </c>
-      <c r="B3" s="33" t="s">
-        <v>813</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>413</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>814</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>415</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>814</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="23" t="s">
-        <v>498</v>
-      </c>
-      <c r="B6" s="33" t="s">
-        <v>814</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="23" t="s">
-        <v>499</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>814</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="220.5">
-      <c r="A8" t="s">
-        <v>801</v>
-      </c>
-      <c r="B8" s="33" t="s">
-        <v>812</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>802</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>812</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>480</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>812</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>803</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>812</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>804</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>815</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="236.25">
-      <c r="A13" s="34" t="s">
-        <v>816</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>812</v>
-      </c>
-      <c r="C13" s="43" t="s">
-        <v>957</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19429,6 +19506,169 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="24.6875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.3125" customWidth="1"/>
+    <col min="3" max="3" width="59.1875" style="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B1" t="s">
+        <v>805</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="315">
+      <c r="A2" t="s">
+        <v>800</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>813</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>814</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>814</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="23" t="s">
+        <v>498</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>814</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="23" t="s">
+        <v>499</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>814</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="220.5">
+      <c r="A8" t="s">
+        <v>801</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>802</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>480</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="C10" s="43" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>803</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>804</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>815</v>
+      </c>
+      <c r="C12" s="43" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="236.25">
+      <c r="A13" s="34" t="s">
+        <v>816</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>812</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>957</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
   <dimension ref="A1:C210"/>
   <sheetViews>
@@ -21741,7 +21981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -21800,7 +22040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -23264,14 +23504,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -23524,6 +23756,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>
@@ -23533,23 +23773,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23566,4 +23789,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating with changes from TBMSL request
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SparrowGIT\Organization-Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84541D56-6842-477A-A89F-29FD29D4BA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D21BB14-F391-46AD-A678-E8ADB11CFF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15511" tabRatio="813" firstSheet="19" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15511" tabRatio="813" firstSheet="19" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4574" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4575" uniqueCount="1123">
   <si>
     <t>Latitude</t>
   </si>
@@ -2829,9 +2829,6 @@
     <t>Tagalog</t>
   </si>
   <si>
-    <t>Grafton - PVA/Joshua</t>
-  </si>
-  <si>
     <t>Grafton - Forut</t>
   </si>
   <si>
@@ -2848,9 +2845,6 @@
   </si>
   <si>
     <t>Grafton - Old camp</t>
-  </si>
-  <si>
-    <t>Grafton - SOJA town</t>
   </si>
   <si>
     <t>Grafton - CRS</t>
@@ -3538,6 +3532,15 @@
   </si>
   <si>
     <t>IPMRN</t>
+  </si>
+  <si>
+    <t>Grafton -  Bai Bureh Ville</t>
+  </si>
+  <si>
+    <t>Grafton - Sorie Bubu</t>
+  </si>
+  <si>
+    <t>Grafton - Hillside</t>
   </si>
 </sst>
 </file>
@@ -3836,7 +3839,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3929,6 +3932,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4429,13 +4435,13 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
@@ -4607,12 +4613,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -4744,12 +4750,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -5358,12 +5364,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
@@ -5903,12 +5909,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6204,12 +6210,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -6449,12 +6455,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>1007</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="51" t="s">
+        <v>1005</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -6481,7 +6487,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="C3" t="s">
         <v>470</v>
@@ -6492,307 +6498,307 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="23" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="23" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="8" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="8" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="8" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="8" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="8" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="8" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="8" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="8" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="8" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="8" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="8" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="8" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="8" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="45" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="45" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="45" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="45" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="45" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="45" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="45" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="45" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="45" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="45" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="45" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="45" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="45" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="45" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="45" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="45" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="45" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="45" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="45" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
     </row>
   </sheetData>
@@ -6825,12 +6831,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>1027</v>
-      </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="53" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -6857,13 +6863,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D3" t="s">
         <v>1028</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1029</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1030</v>
       </c>
       <c r="E3" t="s">
         <v>408</v>
@@ -6871,7 +6877,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="C4" t="s">
         <v>501</v>
@@ -6885,10 +6891,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="C5" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D5" t="s">
         <v>344</v>
@@ -6899,13 +6905,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="C6" t="s">
         <v>503</v>
       </c>
       <c r="D6" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="E6" t="s">
         <v>482</v>
@@ -6913,7 +6919,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="C7" t="s">
         <v>341</v>
@@ -6927,7 +6933,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="C8" t="s">
         <v>470</v>
@@ -6938,7 +6944,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="C9" t="s">
         <v>588</v>
@@ -6949,7 +6955,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -6960,17 +6966,17 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
   </sheetData>
@@ -7015,17 +7021,17 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>1070</v>
-      </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="53" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -7047,13 +7053,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="E3" t="s">
         <v>408</v>
@@ -7061,10 +7067,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>103</v>
@@ -7075,13 +7081,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="E5" t="s">
         <v>410</v>
@@ -7089,121 +7095,121 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
   </sheetData>
@@ -7245,12 +7251,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>855</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7579,12 +7585,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -7840,12 +7846,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -8017,12 +8023,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -8198,12 +8204,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -8580,12 +8586,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -8707,12 +8713,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>933</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="51" t="s">
+        <v>931</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -8733,7 +8739,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="46" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -8750,7 +8756,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="47" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="18" t="s">
@@ -8762,7 +8768,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="47" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="18" t="s">
@@ -8774,7 +8780,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="47" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="18" t="s">
@@ -8786,7 +8792,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="47" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
@@ -8798,7 +8804,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="48" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
@@ -8807,7 +8813,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="48" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
@@ -8816,64 +8822,64 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="48" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="48" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="48" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="48" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="45" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="45" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="45" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="45" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="45" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B19" s="3"/>
     </row>
@@ -8942,12 +8948,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>932</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="51" t="s">
+        <v>930</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -8968,7 +8974,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="46" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -8985,7 +8991,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="47" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="18" t="s">
@@ -8997,7 +9003,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="47" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="18" t="s">
@@ -9009,7 +9015,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="47" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="18" t="s">
@@ -9021,7 +9027,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="47" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
@@ -9033,7 +9039,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="48" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
@@ -9042,7 +9048,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="48" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
@@ -9051,40 +9057,40 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="48" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="48" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="45" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="45" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="45" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B15" s="3"/>
     </row>
@@ -9168,12 +9174,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -9309,15 +9315,15 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.8125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9325,12 +9331,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>883</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -9409,57 +9415,62 @@
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="39" t="s">
-        <v>913</v>
+      <c r="A8" s="50" t="s">
+        <v>1120</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="39" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="39" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="39" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="39" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="39" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="39" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="39" t="s">
-        <v>920</v>
+      <c r="A15" s="50" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="39" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="39" t="s">
-        <v>922</v>
+        <v>920</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="50" t="s">
+        <v>1122</v>
       </c>
     </row>
   </sheetData>
@@ -9501,12 +9512,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -9676,12 +9687,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -9852,12 +9863,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -10028,12 +10039,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="20" t="s">
@@ -19158,17 +19169,17 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>1120</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="51" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -19190,7 +19201,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -19207,7 +19218,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
@@ -19219,7 +19230,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="5" t="s">
@@ -19231,7 +19242,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="4" t="s">
@@ -19240,19 +19251,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -19286,8 +19297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE12B2DA-285C-4280-B25B-5772326A0B3F}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -19299,17 +19310,17 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
-        <v>1121</v>
-      </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="B1" s="51" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -19331,7 +19342,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -19348,7 +19359,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
@@ -19360,7 +19371,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="5" t="s">
@@ -19372,7 +19383,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="4" t="s">
@@ -19381,13 +19392,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="B8" s="3"/>
     </row>
@@ -19451,10 +19462,10 @@
         <v>800</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -19517,10 +19528,10 @@
         <v>801</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -19531,7 +19542,7 @@
         <v>811</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -19575,7 +19586,7 @@
         <v>811</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
   </sheetData>
@@ -19639,7 +19650,7 @@
         <v>842</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -19650,7 +19661,7 @@
         <v>842</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -19661,7 +19672,7 @@
         <v>842</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -19683,7 +19694,7 @@
         <v>842</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -19694,7 +19705,7 @@
         <v>842</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -19716,7 +19727,7 @@
         <v>842</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -19727,7 +19738,7 @@
         <v>842</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -19749,7 +19760,7 @@
         <v>842</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -19760,7 +19771,7 @@
         <v>842</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -19793,7 +19804,7 @@
         <v>842</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -19848,7 +19859,7 @@
         <v>842</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -19859,7 +19870,7 @@
         <v>842</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -19870,7 +19881,7 @@
         <v>842</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -19881,7 +19892,7 @@
         <v>842</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -19903,7 +19914,7 @@
         <v>842</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -20134,7 +20145,7 @@
         <v>842</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -20145,7 +20156,7 @@
         <v>842</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -20352,7 +20363,7 @@
         <v>844</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -20363,7 +20374,7 @@
         <v>844</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25">
@@ -20374,7 +20385,7 @@
         <v>844</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="47.25">
@@ -20385,7 +20396,7 @@
         <v>844</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25">
@@ -20396,7 +20407,7 @@
         <v>844</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="47.25">
@@ -20407,7 +20418,7 @@
         <v>844</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="47.25">
@@ -20418,7 +20429,7 @@
         <v>844</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -20440,7 +20451,7 @@
         <v>844</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -20517,7 +20528,7 @@
         <v>844</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -20528,7 +20539,7 @@
         <v>844</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5">
@@ -20539,7 +20550,7 @@
         <v>844</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="31.5">
@@ -20550,7 +20561,7 @@
         <v>844</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="31.5">
@@ -20561,7 +20572,7 @@
         <v>844</v>
       </c>
       <c r="C90" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="31.5">
@@ -20572,7 +20583,7 @@
         <v>844</v>
       </c>
       <c r="C91" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="31.5">
@@ -20583,7 +20594,7 @@
         <v>844</v>
       </c>
       <c r="C92" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="31.5">
@@ -20594,7 +20605,7 @@
         <v>844</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="31.5">
@@ -20605,7 +20616,7 @@
         <v>844</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="31.5">
@@ -20616,7 +20627,7 @@
         <v>844</v>
       </c>
       <c r="C95" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="31.5">
@@ -20627,7 +20638,7 @@
         <v>844</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="31.5">
@@ -20638,7 +20649,7 @@
         <v>844</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="31.5">
@@ -20649,7 +20660,7 @@
         <v>844</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="31.5">
@@ -20660,7 +20671,7 @@
         <v>844</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="31.5">
@@ -20671,7 +20682,7 @@
         <v>844</v>
       </c>
       <c r="C100" s="42" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -20902,7 +20913,7 @@
         <v>844</v>
       </c>
       <c r="C121" s="42" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -20913,7 +20924,7 @@
         <v>844</v>
       </c>
       <c r="C122" s="42" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -20924,7 +20935,7 @@
         <v>844</v>
       </c>
       <c r="C123" s="42" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -20979,7 +20990,7 @@
         <v>844</v>
       </c>
       <c r="C128" s="42" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -20990,7 +21001,7 @@
         <v>844</v>
       </c>
       <c r="C129" s="42" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -21045,7 +21056,7 @@
         <v>844</v>
       </c>
       <c r="C134" s="42" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -21067,7 +21078,7 @@
         <v>844</v>
       </c>
       <c r="C136" s="42" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -21089,7 +21100,7 @@
         <v>844</v>
       </c>
       <c r="C138" s="42" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -21144,7 +21155,7 @@
         <v>844</v>
       </c>
       <c r="C143" s="42" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -21199,7 +21210,7 @@
         <v>844</v>
       </c>
       <c r="C148" s="42" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -21221,7 +21232,7 @@
         <v>844</v>
       </c>
       <c r="C150" s="42" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -21232,7 +21243,7 @@
         <v>844</v>
       </c>
       <c r="C151" s="42" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -21243,7 +21254,7 @@
         <v>844</v>
       </c>
       <c r="C152" s="42" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -21375,7 +21386,7 @@
         <v>844</v>
       </c>
       <c r="C164" s="42" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -21397,7 +21408,7 @@
         <v>844</v>
       </c>
       <c r="C166" s="42" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -21507,7 +21518,7 @@
         <v>844</v>
       </c>
       <c r="C176" s="42" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -21551,7 +21562,7 @@
         <v>844</v>
       </c>
       <c r="C180" s="42" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -21820,68 +21831,68 @@
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="26" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B205" s="26" t="s">
         <v>844</v>
       </c>
       <c r="C205" s="49" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="26" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="B206" s="26" t="s">
         <v>844</v>
       </c>
       <c r="C206" s="49" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="26" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="B207" s="26" t="s">
         <v>844</v>
       </c>
       <c r="C207" s="49" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="26" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="B208" s="26" t="s">
         <v>844</v>
       </c>
       <c r="C208" s="49" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="26" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B209" s="26" t="s">
         <v>844</v>
       </c>
       <c r="C209" s="49" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="26" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="B210" s="26" t="s">
         <v>844</v>
       </c>
       <c r="C210" s="49" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
   </sheetData>
@@ -22124,12 +22135,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>704</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -22410,12 +22421,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>861</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -22608,12 +22619,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>894</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -22781,12 +22792,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -22963,12 +22974,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -23113,12 +23124,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="19" t="s">
@@ -23418,20 +23429,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23688,6 +23699,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -23700,14 +23719,6 @@
     <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Adding Kingdom Ventures Campaigns
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SparrowGIT\Organization-Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D21BB14-F391-46AD-A678-E8ADB11CFF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57033E8-4869-4BA3-8F37-7B00F7DF5A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15511" tabRatio="813" firstSheet="19" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15495" tabRatio="813" firstSheet="16" activeTab="29" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -41,23 +41,27 @@
     <sheet name="TBMSL" sheetId="40" r:id="rId26"/>
     <sheet name="Go_Build_Love" sheetId="17" r:id="rId27"/>
     <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId28"/>
-    <sheet name="Serve_Hope" sheetId="21" r:id="rId29"/>
-    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId30"/>
-    <sheet name="IPMRP" sheetId="45" r:id="rId31"/>
-    <sheet name="IPMRN" sheetId="46" r:id="rId32"/>
-    <sheet name="Wifi_Materials" sheetId="37" r:id="rId33"/>
-    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId34"/>
-    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId35"/>
-    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId36"/>
+    <sheet name="KVMT" sheetId="47" r:id="rId29"/>
+    <sheet name="KVMR" sheetId="48" r:id="rId30"/>
+    <sheet name="Serve_Hope" sheetId="21" r:id="rId31"/>
+    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId32"/>
+    <sheet name="IPMRP" sheetId="45" r:id="rId33"/>
+    <sheet name="IPMRN" sheetId="46" r:id="rId34"/>
+    <sheet name="Wifi_Materials" sheetId="37" r:id="rId35"/>
+    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId36"/>
+    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId37"/>
+    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId38"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId37"/>
+    <externalReference r:id="rId39"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="29" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="31" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
     <definedName name="Reserved" localSheetId="26">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="27">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="29">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="28">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="30">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="0">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="1">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="2">[1]!tblReserved[Reserved keywords]</definedName>
@@ -87,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4575" uniqueCount="1123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4617" uniqueCount="1125">
   <si>
     <t>Latitude</t>
   </si>
@@ -3541,6 +3545,12 @@
   </si>
   <si>
     <t>Grafton - Hillside</t>
+  </si>
+  <si>
+    <t>Kingdom Ventures Matses Tribe</t>
+  </si>
+  <si>
+    <t>Kingdom Ventures Momon River</t>
   </si>
 </sst>
 </file>
@@ -7004,7 +7014,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -9317,7 +9327,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
@@ -9845,32 +9855,34 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8966E3F0-5F1C-45DE-88BD-0792C7795602}">
-  <dimension ref="A1:E27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B04EE-2E1F-4050-B34E-0DBBEA1DCE38}">
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>32</v>
+        <v>1123</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
       <c r="E1" s="51"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="19" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="19" t="s">
         <v>27</v>
       </c>
@@ -9887,7 +9899,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -9904,7 +9916,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
         <v>118</v>
@@ -9913,7 +9925,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="B5" s="3"/>
       <c r="D5" s="5" t="s">
         <v>119</v>
@@ -9922,49 +9934,49 @@
         <v>410</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="B6" s="2"/>
       <c r="D6" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="2:2">
@@ -10008,7 +10020,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E1623D5B-9BC4-40B7-BC8D-FC4924A27C94}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B6E6C077-DF09-4476-9B80-4681692AD7D0}">
           <x14:formula1>
             <xm:f>Validation!$B$1:$B$5</xm:f>
           </x14:formula1>
@@ -10225,6 +10237,360 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79F542E-5CE0-43CC-9469-549164091111}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="19" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="2"/>
+      <c r="D6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A6F31CD-FD8E-4A6D-888E-AA2C22257E6B}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8966E3F0-5F1C-45DE-88BD-0792C7795602}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="2"/>
+      <c r="D6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E1623D5B-9BC4-40B7-BC8D-FC4924A27C94}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}">
   <dimension ref="A1:D636"/>
   <sheetViews>
@@ -19152,7 +19518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902D9A4C-CB6C-496C-ACF1-A89C91AD596C}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -19293,7 +19659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE12B2DA-285C-4280-B25B-5772326A0B3F}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -19431,7 +19797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -19594,7 +19960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
   <dimension ref="A1:C210"/>
   <sheetViews>
@@ -21909,7 +22275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -21968,7 +22334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -23429,23 +23795,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -23698,10 +24047,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -23724,20 +24101,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding more villages to tbmks campaign
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SparrowGIT\Organization-Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F474AF9-739B-43DE-8AE9-B0266A1E0234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58982300-5BCE-43FE-8154-EC10FA120FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15481" tabRatio="813" firstSheet="16" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15481" tabRatio="813" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4638" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4672" uniqueCount="1181">
   <si>
     <t>Latitude</t>
   </si>
@@ -3617,6 +3617,108 @@
   </si>
   <si>
     <t>Peru</t>
+  </si>
+  <si>
+    <t>Entasopia - Idakalani A</t>
+  </si>
+  <si>
+    <t>Entasopia - Idakalani B</t>
+  </si>
+  <si>
+    <t>Entasopia - Konei A</t>
+  </si>
+  <si>
+    <t>Entasopia - Konei B</t>
+  </si>
+  <si>
+    <t>Entasopia - Soweto</t>
+  </si>
+  <si>
+    <t>Entasopia - Entasopia</t>
+  </si>
+  <si>
+    <t>Entasopia - Osopuko</t>
+  </si>
+  <si>
+    <t>Entasopia - Olkeres</t>
+  </si>
+  <si>
+    <t>Entasopia - Entumoto</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Ololelai</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Israel A</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Israel B</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Entasopia intake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olchoro olepo - Olodungoro </t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Olchoro oirobi</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Olchoro olepo</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Naserian</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - K.A.G</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Imani</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Tenebo</t>
+  </si>
+  <si>
+    <t>Olchoro olepo - Bondeni</t>
+  </si>
+  <si>
+    <t>Ngurman - Oltarañja</t>
+  </si>
+  <si>
+    <t>Ngurman - Mokinyo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngurman - Osupuko </t>
+  </si>
+  <si>
+    <t>Ngurman - Empeut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngurman - Olngarua </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngurman - Esonorua </t>
+  </si>
+  <si>
+    <t>Ngurman - Kongo</t>
+  </si>
+  <si>
+    <t>Ngurman - Oltepesi</t>
+  </si>
+  <si>
+    <t>Ngurman - Olomelok</t>
+  </si>
+  <si>
+    <t>Ngurman - Kamorora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngurman - Olboirtoto Primary </t>
+  </si>
+  <si>
+    <t>Ngurman - Intake 1</t>
+  </si>
+  <si>
+    <t>Ngurman - Intake 2</t>
   </si>
 </sst>
 </file>
@@ -6512,15 +6614,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39F5EFB-4C75-4F45-95CF-B50496BF741C}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A40" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.6875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6875" style="43" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.8125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6875" bestFit="1" customWidth="1"/>
@@ -6528,7 +6630,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
@@ -6545,7 +6647,7 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -6562,7 +6664,7 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
+      <c r="A3" s="43" t="s">
         <v>962</v>
       </c>
       <c r="C3" t="s">
@@ -6573,308 +6675,478 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
+      <c r="A4" s="43" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
+      <c r="A5" s="43" t="s">
         <v>964</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="43" t="s">
         <v>965</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="43" t="s">
         <v>966</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
+      <c r="A8" s="43" t="s">
         <v>967</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
+      <c r="A9" s="43" t="s">
         <v>968</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="A10" s="43" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="A11" s="43" t="s">
         <v>970</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" t="s">
+      <c r="A12" s="43" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" t="s">
+      <c r="A13" s="43" t="s">
         <v>972</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
+      <c r="A14" s="43" t="s">
         <v>973</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" t="s">
+      <c r="A15" s="43" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="A16" s="43" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="A17" s="43" t="s">
         <v>976</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="A18" s="43" t="s">
         <v>977</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="A19" s="43" t="s">
         <v>978</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="A20" s="43" t="s">
         <v>979</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" t="s">
+      <c r="A21" s="43" t="s">
         <v>980</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" t="s">
+      <c r="A22" s="43" t="s">
         <v>981</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" t="s">
+      <c r="A23" s="43" t="s">
         <v>982</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" t="s">
+      <c r="A24" s="43" t="s">
         <v>983</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" t="s">
+      <c r="A25" s="43" t="s">
         <v>984</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="A26" s="43" t="s">
         <v>985</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="A27" s="43" t="s">
         <v>986</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" t="s">
+      <c r="A28" s="43" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" t="s">
+      <c r="A29" s="43" t="s">
         <v>988</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" t="s">
+      <c r="A30" s="43" t="s">
         <v>989</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" t="s">
+      <c r="A31" s="43" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="A32" s="43" t="s">
         <v>991</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="43" t="s">
         <v>992</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="43" t="s">
         <v>993</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="43" t="s">
         <v>994</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="43" t="s">
         <v>995</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="43" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="43" t="s">
         <v>997</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="43" t="s">
         <v>998</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="43" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="43" t="s">
         <v>1000</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="43" t="s">
         <v>1001</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="43" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="43" t="s">
         <v>1003</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="43" t="s">
         <v>1004</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="45" t="s">
+      <c r="A46" s="43" t="s">
         <v>1006</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="45" t="s">
+      <c r="A47" s="43" t="s">
         <v>1007</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="45" t="s">
+      <c r="A48" s="43" t="s">
         <v>1008</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="45" t="s">
+      <c r="A49" s="43" t="s">
         <v>1009</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="45" t="s">
+      <c r="A50" s="43" t="s">
         <v>1010</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="45" t="s">
+      <c r="A51" s="43" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="45" t="s">
+      <c r="A52" s="43" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="45" t="s">
+      <c r="A53" s="43" t="s">
         <v>1013</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="45" t="s">
+      <c r="A54" s="43" t="s">
         <v>1014</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="43" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="45" t="s">
+      <c r="A56" s="43" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="45" t="s">
+      <c r="A57" s="43" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="45" t="s">
+      <c r="A58" s="43" t="s">
         <v>1018</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="45" t="s">
+      <c r="A59" s="43" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="45" t="s">
+      <c r="A60" s="43" t="s">
         <v>1020</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="45" t="s">
+      <c r="A61" s="43" t="s">
         <v>1021</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="45" t="s">
+      <c r="A62" s="43" t="s">
         <v>1022</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="43" t="s">
         <v>1023</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="45" t="s">
+      <c r="A64" s="43" t="s">
         <v>1024</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="43" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="43" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="43" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="43" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="43" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="43" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="43" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="43" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="43" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="43" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="43" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="43" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="43" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="43" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="43" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="43" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="43" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="43" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="43" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="43" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="43" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="43" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="43" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="43" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="43" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="43" t="s">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="43" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="43" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="43" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="43" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="43" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="43" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="43" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="43" t="s">
+        <v>1180</v>
       </c>
     </row>
   </sheetData>
@@ -9924,7 +10196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B04EE-2E1F-4050-B34E-0DBBEA1DCE38}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -23924,23 +24196,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -24193,10 +24448,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24219,20 +24502,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating with changes from Victor
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SparrowGIT\Organization-Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SparrowGIT\TBM_Organization_Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01F77FD-C755-4ADC-988D-A2547960109E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3434C38-33CB-4785-B5F2-4C9282964976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15481" tabRatio="813" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4723" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4723" uniqueCount="1207">
   <si>
     <t>Latitude</t>
   </si>
@@ -2879,9 +2879,6 @@
     <t>Afrikaans, IsiXhosa, IsiZulu, Ndebele Northern,</t>
   </si>
   <si>
-    <t>Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, Baniwa, Banjara, Bengali, Bono, Bora, Buji, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Konkomba, Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lumasaba, Lunyankore, Lusamya, Luyole, Magogo, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nchumburu, Ngas, Nhengatu, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sisaali, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
-  </si>
-  <si>
     <t>Afrikaans, English, Kiswahili, Portuguese, Spanish,</t>
   </si>
   <si>
@@ -3644,9 +3641,6 @@
     <t>Abaganda</t>
   </si>
   <si>
-    <t>LuSamia</t>
-  </si>
-  <si>
     <t>Abasamia</t>
   </si>
   <si>
@@ -3692,9 +3686,6 @@
     <t>Namakoli Nambengele B</t>
   </si>
   <si>
-    <t>TBM, TBMAR, TBMCV, TBMKA, TBMK, TBMPB</t>
-  </si>
-  <si>
     <t xml:space="preserve">Acholi, Adele, Afrikaans, Akan-Akuapem-Twi, Akan-Asante, Akan-Fante, Alur, Anufo, Ateso, Bimoba, Birifor-Southern, Borana, Buli, Canela, Chumburung, Daasanach, Dagaare, Dagbani, Dhopadhola, Duruma, English, Ewe, Ga, Gikyode, Giryama, Guajajara, Hanga, Ilchamus, IsiXhosa, IsiZulu, Kaapor, Kadiweu, Kakwa, Kalenjin, Kamba, Karimojong, Kasem, Kayabi, Kayapo,  Kebu, Kikamba, Kimeru, Kiswahili, Kiwihwana, Koma, Konkomba-Likoonli, Konkomba-Likpakpaaln, Kumam, Kupsapiny, Kusaal, Lango, Lelemi, Lubwisi, Luganda, Lugbara, Lumasaaba, Lunyore, Luo, Lusoga, Maasai, Madi, Mampruli, Meru, Ndebele Northern, Ndebele Southern, Nkonya, Nzema, Paasaal, Parecis, Polkoot, Portuguese, Runyankore, Runyoro-Rutoro, Sabaot, Samburu, Sisaala-Tumulung, siSwati, Sesotho, Sesotho sa Leboa, Setswana, Spanish, Suba, Taita, Tampulma, Tharaka, Turkana, Vagla, Wali, Xitsonga, Cebuano </t>
   </si>
   <si>
@@ -3711,6 +3702,170 @@
   </si>
   <si>
     <t>Afrikaans, English, IsiXhosa, IsiZulu, Ndebele Northern, Portuguese, Setswana, siSwati, Cebuano</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TBM, TBMAR, TBMCV, TBMKA, TBMK, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TBMKB</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TBM, TBMAR, TBMCV, TBMKA, TBMK, TBMPB, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TBMKB,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bakhayo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Baniwa, Banjara, Bengali, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Banyore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Bono, Bora, Buji, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Dholuo, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Giriama</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Konkomba, Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lumasaba, Lunyankore, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">LuSamia, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Luyole, Magogo, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Marachi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nchumburu, Ngas, Nhengatu, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sisaali, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">TBM, TBMAR, TBMCV, TBMKA, TBMK, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TBMKB,</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6950,7 +7105,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -6981,7 +7136,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="43" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C3" t="s">
         <v>470</v>
@@ -6992,502 +7147,502 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="43" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="43" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="43" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="43" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="43" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="43" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="43" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="43" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="43" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="43" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="43" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="43" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="43" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="43" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="43" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="43" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="43" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="43" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="43" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="43" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="43" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="43" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="43" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="43" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="43" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="43" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="43" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="43" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="43" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="43" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="43" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="43" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="43" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="43" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="43" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="43" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="43" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="43" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="43" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="43" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="43" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="43" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="43" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="43" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="43" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="43" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="43" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="43" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="43" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" s="43" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="43" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="43" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" s="43" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" s="43" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" s="43" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" s="43" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" s="43" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" s="43" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" s="43" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" s="43" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="43" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="43" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="43" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="43" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="43" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="43" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="43" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="43" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="43" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="43" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="43" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="43" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="43" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="43" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="43" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="43" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="43" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="43" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="43" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="43" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="43" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="43" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="43" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="43" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="43" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="43" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="43" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="43" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="43" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="43" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="43" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="43" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="43" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="43" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="43" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="43" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="43" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="43" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="43" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="43" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
   </sheetData>
@@ -7521,7 +7676,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C1" s="52"/>
       <c r="D1" s="52"/>
@@ -7552,13 +7707,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C3" t="s">
         <v>1026</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1027</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1028</v>
       </c>
       <c r="E3" t="s">
         <v>408</v>
@@ -7566,7 +7721,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="C4" t="s">
         <v>501</v>
@@ -7580,10 +7735,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C5" t="s">
         <v>1030</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1031</v>
       </c>
       <c r="D5" t="s">
         <v>344</v>
@@ -7594,13 +7749,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C6" t="s">
         <v>503</v>
       </c>
       <c r="D6" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="E6" t="s">
         <v>482</v>
@@ -7608,7 +7763,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C7" t="s">
         <v>341</v>
@@ -7622,7 +7777,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C8" t="s">
         <v>470</v>
@@ -7633,7 +7788,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="C9" t="s">
         <v>588</v>
@@ -7644,7 +7799,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -7655,17 +7810,17 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
     </row>
   </sheetData>
@@ -7711,7 +7866,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C1" s="52"/>
       <c r="D1" s="52"/>
@@ -7720,7 +7875,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -7742,13 +7897,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E3" t="s">
         <v>408</v>
@@ -7756,10 +7911,10 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D4" s="27" t="s">
         <v>103</v>
@@ -7770,13 +7925,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="E5" t="s">
         <v>410</v>
@@ -7784,121 +7939,121 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
     </row>
   </sheetData>
@@ -9403,7 +9558,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -9428,7 +9583,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="46" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -9445,7 +9600,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="47" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="18" t="s">
@@ -9457,7 +9612,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="47" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="18" t="s">
@@ -9469,7 +9624,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="47" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="18" t="s">
@@ -9481,7 +9636,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="47" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
@@ -9493,7 +9648,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="48" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
@@ -9502,7 +9657,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="48" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
@@ -9511,64 +9666,64 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="48" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="48" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="48" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="48" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="45" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="45" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="45" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="45" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="45" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B19" s="3"/>
     </row>
@@ -9638,7 +9793,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -9663,7 +9818,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="46" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -9680,7 +9835,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="47" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="18" t="s">
@@ -9692,7 +9847,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="47" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="18" t="s">
@@ -9704,7 +9859,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="47" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="18" t="s">
@@ -9716,7 +9871,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="47" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
@@ -9728,7 +9883,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="48" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
@@ -9737,7 +9892,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="48" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
@@ -9746,40 +9901,40 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="48" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="48" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="48" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="45" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="45" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="45" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B15" s="3"/>
     </row>
@@ -10105,7 +10260,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="50" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4"/>
@@ -10144,7 +10299,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="50" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -10159,7 +10314,7 @@
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="50" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -10756,7 +10911,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -10765,7 +10920,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -10787,7 +10942,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -10804,7 +10959,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
@@ -10940,7 +11095,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -10949,7 +11104,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -10971,7 +11126,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -10988,7 +11143,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
@@ -11000,7 +11155,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="5" t="s">
@@ -11012,7 +11167,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="4" t="s">
@@ -11021,7 +11176,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
@@ -11030,7 +11185,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
@@ -11039,7 +11194,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
@@ -11048,73 +11203,73 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B21" s="3"/>
     </row>
@@ -20278,7 +20433,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -20287,7 +20442,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -20309,7 +20464,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -20326,7 +20481,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
@@ -20338,7 +20493,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="5" t="s">
@@ -20350,7 +20505,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="4" t="s">
@@ -20359,19 +20514,19 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B9" s="3"/>
     </row>
@@ -20419,7 +20574,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="C1" s="51"/>
       <c r="D1" s="51"/>
@@ -20428,7 +20583,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -20450,7 +20605,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
@@ -20467,7 +20622,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B4" s="3"/>
       <c r="D4" s="4" t="s">
@@ -20479,7 +20634,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="5" t="s">
@@ -20491,7 +20646,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="4" t="s">
@@ -20500,25 +20655,25 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="B10" s="3"/>
     </row>
@@ -20550,7 +20705,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
@@ -20576,10 +20731,10 @@
         <v>800</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>1199</v>
+        <v>1204</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -20642,21 +20797,21 @@
         <v>801</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>1199</v>
+        <v>1204</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="31.5">
       <c r="A9" t="s">
         <v>802</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>811</v>
+        <v>1206</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -20692,15 +20847,15 @@
         <v>810</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="236.25">
+    <row r="13" spans="1:3" ht="252">
       <c r="A13" s="34" t="s">
         <v>815</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>811</v>
+        <v>1203</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>928</v>
+        <v>1205</v>
       </c>
     </row>
   </sheetData>
@@ -20764,7 +20919,7 @@
         <v>842</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -20775,7 +20930,7 @@
         <v>842</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -20786,7 +20941,7 @@
         <v>842</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -20808,7 +20963,7 @@
         <v>842</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -20819,7 +20974,7 @@
         <v>842</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -20841,7 +20996,7 @@
         <v>842</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -20852,7 +21007,7 @@
         <v>842</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -20874,7 +21029,7 @@
         <v>842</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -20885,7 +21040,7 @@
         <v>842</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -20918,7 +21073,7 @@
         <v>842</v>
       </c>
       <c r="C18" s="42" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -20973,7 +21128,7 @@
         <v>842</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -20984,7 +21139,7 @@
         <v>842</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -20995,7 +21150,7 @@
         <v>842</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -21006,7 +21161,7 @@
         <v>842</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -21028,7 +21183,7 @@
         <v>842</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -21259,7 +21414,7 @@
         <v>842</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -21270,7 +21425,7 @@
         <v>842</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -21477,7 +21632,7 @@
         <v>844</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -21488,7 +21643,7 @@
         <v>844</v>
       </c>
       <c r="C72" s="42" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="47.25">
@@ -21499,7 +21654,7 @@
         <v>844</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="47.25">
@@ -21510,7 +21665,7 @@
         <v>844</v>
       </c>
       <c r="C74" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="47.25">
@@ -21521,7 +21676,7 @@
         <v>844</v>
       </c>
       <c r="C75" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="47.25">
@@ -21532,7 +21687,7 @@
         <v>844</v>
       </c>
       <c r="C76" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="47.25">
@@ -21543,7 +21698,7 @@
         <v>844</v>
       </c>
       <c r="C77" s="42" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -21565,7 +21720,7 @@
         <v>844</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -21642,7 +21797,7 @@
         <v>844</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -21653,7 +21808,7 @@
         <v>844</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5">
@@ -21664,7 +21819,7 @@
         <v>844</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="31.5">
@@ -21675,7 +21830,7 @@
         <v>844</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="31.5">
@@ -21686,7 +21841,7 @@
         <v>844</v>
       </c>
       <c r="C90" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="31.5">
@@ -21697,7 +21852,7 @@
         <v>844</v>
       </c>
       <c r="C91" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="31.5">
@@ -21708,7 +21863,7 @@
         <v>844</v>
       </c>
       <c r="C92" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="31.5">
@@ -21719,7 +21874,7 @@
         <v>844</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="31.5">
@@ -21730,7 +21885,7 @@
         <v>844</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="31.5">
@@ -21741,7 +21896,7 @@
         <v>844</v>
       </c>
       <c r="C95" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="31.5">
@@ -21752,7 +21907,7 @@
         <v>844</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="31.5">
@@ -21763,7 +21918,7 @@
         <v>844</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="31.5">
@@ -21774,7 +21929,7 @@
         <v>844</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="31.5">
@@ -21785,7 +21940,7 @@
         <v>844</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="31.5">
@@ -21796,7 +21951,7 @@
         <v>844</v>
       </c>
       <c r="C100" s="42" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -22027,7 +22182,7 @@
         <v>844</v>
       </c>
       <c r="C121" s="42" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -22038,7 +22193,7 @@
         <v>844</v>
       </c>
       <c r="C122" s="42" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -22049,7 +22204,7 @@
         <v>844</v>
       </c>
       <c r="C123" s="42" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -22104,7 +22259,7 @@
         <v>844</v>
       </c>
       <c r="C128" s="42" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="129" spans="1:3">
@@ -22115,7 +22270,7 @@
         <v>844</v>
       </c>
       <c r="C129" s="42" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="130" spans="1:3">
@@ -22170,7 +22325,7 @@
         <v>844</v>
       </c>
       <c r="C134" s="42" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -22192,7 +22347,7 @@
         <v>844</v>
       </c>
       <c r="C136" s="42" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="137" spans="1:3">
@@ -22214,7 +22369,7 @@
         <v>844</v>
       </c>
       <c r="C138" s="42" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="139" spans="1:3">
@@ -22269,7 +22424,7 @@
         <v>844</v>
       </c>
       <c r="C143" s="42" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="144" spans="1:3">
@@ -22324,7 +22479,7 @@
         <v>844</v>
       </c>
       <c r="C148" s="42" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="149" spans="1:3">
@@ -22346,7 +22501,7 @@
         <v>844</v>
       </c>
       <c r="C150" s="42" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="151" spans="1:3">
@@ -22357,7 +22512,7 @@
         <v>844</v>
       </c>
       <c r="C151" s="42" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="152" spans="1:3">
@@ -22368,7 +22523,7 @@
         <v>844</v>
       </c>
       <c r="C152" s="42" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="153" spans="1:3">
@@ -22500,7 +22655,7 @@
         <v>844</v>
       </c>
       <c r="C164" s="42" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -22522,7 +22677,7 @@
         <v>844</v>
       </c>
       <c r="C166" s="42" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -22632,7 +22787,7 @@
         <v>844</v>
       </c>
       <c r="C176" s="42" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -22676,7 +22831,7 @@
         <v>844</v>
       </c>
       <c r="C180" s="42" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -23519,7 +23674,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D3" sqref="D3:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -23537,7 +23692,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C1" s="52"/>
       <c r="D1" s="52"/>
@@ -23568,13 +23723,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="C3" t="s">
         <v>469</v>
       </c>
-      <c r="D3" t="s">
-        <v>1028</v>
+      <c r="D3" s="8" t="s">
+        <v>469</v>
       </c>
       <c r="E3" t="s">
         <v>408</v>
@@ -23582,12 +23737,12 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
       <c r="C4" t="s">
         <v>340</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="8" t="s">
         <v>340</v>
       </c>
       <c r="E4" t="s">
@@ -23596,13 +23751,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
       <c r="C5" t="s">
-        <v>1182</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1183</v>
+        <v>1181</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>563</v>
       </c>
       <c r="E5" t="s">
         <v>410</v>
@@ -23610,13 +23765,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1193</v>
+        <v>1191</v>
       </c>
       <c r="C6" t="s">
-        <v>1184</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1185</v>
+        <v>1182</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>1183</v>
       </c>
       <c r="E6" t="s">
         <v>482</v>
@@ -23624,13 +23779,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="C7" t="s">
-        <v>1186</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1187</v>
+        <v>1184</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>1185</v>
       </c>
       <c r="E7" t="s">
         <v>481</v>
@@ -23638,45 +23793,45 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1195</v>
+        <v>1193</v>
       </c>
       <c r="C8" t="s">
-        <v>1188</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1189</v>
+        <v>1186</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>1187</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="C9" t="s">
         <v>503</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="8" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="C10" t="s">
         <v>342</v>
       </c>
-      <c r="D10" t="s">
-        <v>587</v>
+      <c r="D10" s="8" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="C11" t="s">
         <v>587</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="8" t="s">
         <v>343</v>
       </c>
     </row>
@@ -23684,7 +23839,7 @@
       <c r="C12" t="s">
         <v>477</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="8" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating with KVMR village updates
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\SparrowGIT\TBM_Organization_Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3434C38-33CB-4785-B5F2-4C9282964976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E3D58F-C5CC-466C-9BE3-D59E6208D97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15481" tabRatio="813" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15481" tabRatio="813" firstSheet="18" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <sheet name="TBMSA" sheetId="31" r:id="rId26"/>
     <sheet name="TBMSL" sheetId="40" r:id="rId27"/>
     <sheet name="Go_Build_Love" sheetId="17" r:id="rId28"/>
-    <sheet name="Kingdom_Ventures" sheetId="30" r:id="rId29"/>
+    <sheet name="Kingdom_Ventures(Disabled)" sheetId="30" r:id="rId29"/>
     <sheet name="KVMT" sheetId="47" r:id="rId30"/>
     <sheet name="KVMR" sheetId="48" r:id="rId31"/>
     <sheet name="Serve_Hope" sheetId="21" r:id="rId32"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4723" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4726" uniqueCount="1210">
   <si>
     <t>Latitude</t>
   </si>
@@ -3465,9 +3465,6 @@
   </si>
   <si>
     <t>Santa Rosa</t>
-  </si>
-  <si>
-    <t>GenGrn</t>
   </si>
   <si>
     <t>Centro Fuerte</t>
@@ -3866,6 +3863,18 @@
       </rPr>
       <t>TBMKB,</t>
     </r>
+  </si>
+  <si>
+    <t>Gen Gen</t>
+  </si>
+  <si>
+    <t>San Juan Polis</t>
+  </si>
+  <si>
+    <t>8 de Setiembre</t>
+  </si>
+  <si>
+    <t>Nuevo Paraíso</t>
   </si>
 </sst>
 </file>
@@ -5998,7 +6007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5B793A-E672-42F0-B7CD-796F921CC77D}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:A50"/>
     </sheetView>
   </sheetViews>
@@ -7452,197 +7461,197 @@
     </row>
     <row r="65" spans="1:1">
       <c r="A65" s="43" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" s="43" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" s="43" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" s="43" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" s="43" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" s="43" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" s="43" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" s="43" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="43" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" s="43" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" s="43" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" s="43" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" s="43" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" s="43" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" s="43" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" s="43" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="43" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" s="43" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" s="43" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" s="43" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" s="43" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" s="43" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" s="43" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" s="43" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" s="43" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="43" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" s="43" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" s="43" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" s="43" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" s="43" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" s="43" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" s="43" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" s="43" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" s="43" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" s="43" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" s="43" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" s="43" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" s="43" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" s="43" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
   </sheetData>
@@ -10920,7 +10929,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -11080,8 +11089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79F542E-5CE0-43CC-9469-549164091111}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75"/>
@@ -11104,7 +11113,7 @@
         <v>496</v>
       </c>
       <c r="G1" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -11184,8 +11193,8 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>1124</v>
+      <c r="A8" s="45" t="s">
+        <v>1206</v>
       </c>
       <c r="B8" s="3"/>
       <c r="D8" s="4" t="s">
@@ -11194,7 +11203,7 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B9" s="3"/>
       <c r="D9" s="4" t="s">
@@ -11203,83 +11212,92 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2">
+      <c r="A22" s="45" t="s">
+        <v>1207</v>
+      </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2">
+      <c r="A23" s="45" t="s">
+        <v>1208</v>
+      </c>
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2">
+      <c r="A24" s="45" t="s">
+        <v>1209</v>
+      </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2">
@@ -20667,13 +20685,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B10" s="3"/>
     </row>
@@ -20731,7 +20749,7 @@
         <v>800</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>1058</v>
@@ -20797,10 +20815,10 @@
         <v>801</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5">
@@ -20808,7 +20826,7 @@
         <v>802</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>928</v>
@@ -20852,10 +20870,10 @@
         <v>815</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
     </row>
   </sheetData>
@@ -21632,7 +21650,7 @@
         <v>844</v>
       </c>
       <c r="C71" s="42" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -21720,7 +21738,7 @@
         <v>844</v>
       </c>
       <c r="C79" s="42" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -21808,7 +21826,7 @@
         <v>844</v>
       </c>
       <c r="C87" s="42" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="31.5">
@@ -21819,7 +21837,7 @@
         <v>844</v>
       </c>
       <c r="C88" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="31.5">
@@ -21830,7 +21848,7 @@
         <v>844</v>
       </c>
       <c r="C89" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="31.5">
@@ -21841,7 +21859,7 @@
         <v>844</v>
       </c>
       <c r="C90" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="31.5">
@@ -21852,7 +21870,7 @@
         <v>844</v>
       </c>
       <c r="C91" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="31.5">
@@ -21863,7 +21881,7 @@
         <v>844</v>
       </c>
       <c r="C92" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="31.5">
@@ -21874,7 +21892,7 @@
         <v>844</v>
       </c>
       <c r="C93" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="31.5">
@@ -21885,7 +21903,7 @@
         <v>844</v>
       </c>
       <c r="C94" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="31.5">
@@ -21896,7 +21914,7 @@
         <v>844</v>
       </c>
       <c r="C95" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="31.5">
@@ -21907,7 +21925,7 @@
         <v>844</v>
       </c>
       <c r="C96" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="31.5">
@@ -21918,7 +21936,7 @@
         <v>844</v>
       </c>
       <c r="C97" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="31.5">
@@ -21929,7 +21947,7 @@
         <v>844</v>
       </c>
       <c r="C98" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="31.5">
@@ -21940,7 +21958,7 @@
         <v>844</v>
       </c>
       <c r="C99" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="31.5">
@@ -21951,7 +21969,7 @@
         <v>844</v>
       </c>
       <c r="C100" s="42" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="101" spans="1:3">
@@ -22677,7 +22695,7 @@
         <v>844</v>
       </c>
       <c r="C166" s="42" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="167" spans="1:3">
@@ -23673,7 +23691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2983EA-E482-40E6-803A-79BDAC338E85}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D12"/>
     </sheetView>
   </sheetViews>
@@ -23692,7 +23710,7 @@
         <v>391</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C1" s="52"/>
       <c r="D1" s="52"/>
@@ -23723,7 +23741,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C3" t="s">
         <v>469</v>
@@ -23737,7 +23755,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C4" t="s">
         <v>340</v>
@@ -23751,10 +23769,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C5" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>563</v>
@@ -23765,13 +23783,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C6" t="s">
+        <v>1181</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>1182</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>1183</v>
       </c>
       <c r="E6" t="s">
         <v>482</v>
@@ -23779,13 +23797,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C7" t="s">
+        <v>1183</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>1184</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>1185</v>
       </c>
       <c r="E7" t="s">
         <v>481</v>
@@ -23793,18 +23811,18 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C8" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>1186</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>1187</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C9" t="s">
         <v>503</v>
@@ -23815,7 +23833,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C10" t="s">
         <v>342</v>
@@ -23826,7 +23844,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C11" t="s">
         <v>587</v>
@@ -24561,14 +24579,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -24821,6 +24831,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24831,23 +24849,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24866,6 +24867,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated with Northern Ghana Villages
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MicroDrive/SparrowGIT/TBM_Organization_Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F803B258-E737-AC4C-8744-7D3FCE303D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A154878B-60FD-724D-9A48-5D17AE26BA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4754" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4751" uniqueCount="1238">
   <si>
     <t>Latitude</t>
   </si>
@@ -3807,25 +3807,30 @@
   <si>
     <t>Iloshon  </t>
   </si>
+  <si>
+    <t>Satani Baatingli</t>
+  </si>
+  <si>
+    <t>Satani Zugsaaya</t>
+  </si>
+  <si>
+    <t>Yilkpani</t>
+  </si>
+  <si>
+    <t>Yipieligu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4053,7 +4058,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4072,12 +4077,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4090,9 +4089,9 @@
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -4104,95 +4103,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4693,13 +4685,13 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -4872,12 +4864,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -5195,12 +5187,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -5332,12 +5324,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -5946,12 +5938,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -6455,7 +6447,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -6491,12 +6483,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -6792,12 +6784,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7020,7 +7012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39F5EFB-4C75-4F45-95CF-B50496BF741C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A104" sqref="A104:A123"/>
     </sheetView>
   </sheetViews>
@@ -7037,12 +7029,12 @@
       <c r="A1" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1001</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -7708,12 +7700,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>1021</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -7898,12 +7890,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>1055</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -8128,12 +8120,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>852</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8461,12 +8453,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8638,12 +8630,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8900,12 +8892,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9081,12 +9073,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="47" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9449,8 +9441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9796B9BC-A579-4EDE-99EB-40D54CC290A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9463,12 +9455,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="47" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9489,66 +9481,60 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>117</v>
+        <v>1234</v>
       </c>
       <c r="B3" t="s">
         <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>103</v>
+        <v>170</v>
       </c>
       <c r="E3" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
+      <c r="A4" s="18" t="s">
+        <v>1235</v>
+      </c>
       <c r="B4" s="3"/>
-      <c r="D4" s="18" t="s">
-        <v>118</v>
-      </c>
+      <c r="D4" s="18"/>
       <c r="E4" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
+      <c r="A5" s="18" t="s">
+        <v>1236</v>
+      </c>
       <c r="B5" s="3"/>
-      <c r="D5" s="18" t="s">
-        <v>119</v>
-      </c>
+      <c r="D5" s="18"/>
       <c r="E5" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="18" t="s">
+        <v>1237</v>
+      </c>
       <c r="B6" s="2"/>
-      <c r="D6" s="18" t="s">
-        <v>104</v>
-      </c>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="18"/>
       <c r="B7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>120</v>
-      </c>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
-      <c r="D8" s="4" t="s">
-        <v>121</v>
-      </c>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9575,7 +9561,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9590,12 +9576,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>927</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9615,7 +9601,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" t="s">
         <v>928</v>
       </c>
       <c r="B3" t="s">
@@ -9632,7 +9618,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="8" t="s">
         <v>929</v>
       </c>
       <c r="B4" s="3"/>
@@ -9644,43 +9630,43 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" t="s">
         <v>930</v>
       </c>
       <c r="B5" s="3"/>
       <c r="D5" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="8" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="8" t="s">
         <v>931</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" s="18" t="s">
         <v>389</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="8" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" t="s">
         <v>932</v>
       </c>
       <c r="B7" s="3"/>
       <c r="D7" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="8" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="8" t="s">
         <v>933</v>
       </c>
       <c r="B8" s="3"/>
@@ -9689,7 +9675,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
+      <c r="A9" t="s">
         <v>934</v>
       </c>
       <c r="B9" s="3"/>
@@ -9698,64 +9684,64 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="8" t="s">
         <v>935</v>
       </c>
       <c r="B10" s="3"/>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" t="s">
         <v>936</v>
       </c>
       <c r="B11" s="3"/>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="8" t="s">
         <v>937</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
+      <c r="A13" t="s">
         <v>938</v>
       </c>
       <c r="B13" s="2"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="8" t="s">
         <v>939</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
+      <c r="A15" t="s">
         <v>940</v>
       </c>
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="8" t="s">
         <v>941</v>
       </c>
       <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="44" t="s">
+      <c r="A17" t="s">
         <v>942</v>
       </c>
       <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="8" t="s">
         <v>943</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="44" t="s">
+      <c r="A19" t="s">
         <v>944</v>
       </c>
       <c r="B19" s="3"/>
@@ -9810,7 +9796,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9825,12 +9811,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>926</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9850,7 +9836,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="45" t="s">
+      <c r="A3" t="s">
         <v>945</v>
       </c>
       <c r="B3" t="s">
@@ -9859,7 +9845,7 @@
       <c r="C3" t="s">
         <v>390</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" t="s">
         <v>119</v>
       </c>
       <c r="E3" t="s">
@@ -9867,11 +9853,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
+      <c r="A4" t="s">
         <v>946</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="18" t="s">
+      <c r="D4" t="s">
         <v>387</v>
       </c>
       <c r="E4" t="s">
@@ -9879,11 +9864,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="46" t="s">
+      <c r="A5" t="s">
         <v>947</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="D5" s="18" t="s">
+      <c r="D5" t="s">
         <v>388</v>
       </c>
       <c r="E5" t="s">
@@ -9891,89 +9875,72 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="46" t="s">
+      <c r="A6" t="s">
         <v>948</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="D6" s="18" t="s">
+      <c r="D6" t="s">
         <v>389</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="46" t="s">
+      <c r="A7" t="s">
         <v>949</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" t="s">
         <v>118</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
+      <c r="A8" t="s">
         <v>950</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
+      <c r="A9" t="s">
         <v>951</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
+      <c r="A10" t="s">
         <v>952</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" t="s">
         <v>953</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" t="s">
         <v>954</v>
       </c>
-      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="44" t="s">
+      <c r="A13" t="s">
         <v>955</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="44" t="s">
+      <c r="A14" t="s">
         <v>956</v>
       </c>
-      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="44" t="s">
+      <c r="A15" t="s">
         <v>957</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="44"/>
@@ -10051,12 +10018,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10209,12 +10176,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>880</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10413,12 +10380,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10588,12 +10555,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10764,12 +10731,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -10967,12 +10934,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1110</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -11151,12 +11118,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1111</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -11398,12 +11365,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -20500,12 +20467,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1105</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -20641,12 +20608,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>1106</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -20915,7 +20882,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="289" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>813</v>
       </c>
@@ -23472,12 +23439,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>704</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -23720,7 +23687,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="18" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -23759,12 +23726,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>1174</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -23945,12 +23912,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>858</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -24143,12 +24110,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="47" t="s">
         <v>891</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -24316,12 +24283,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -24498,12 +24465,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -24629,6 +24596,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -24881,14 +24856,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24899,6 +24866,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24917,23 +24901,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Finishing update with null data in wifi
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MicroDrive/SparrowGIT/TBM_Organization_Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A4A9A5-3B47-0945-8EEB-641BDB23D01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8BE4BA-EDB9-AD4E-A7D9-EDF1A0CF4E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="21" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="21" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -5342,28 +5342,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, Bakhayo, Baniwa, Banjara, Bengali, Banyore, Bono, Bora, Buji, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, Dholuo, Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, Giriama, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Konkomba, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">Komo, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lumasaba, Lunyankore, LuSamia, Luyole, Magogo, Marachi, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nchumburu, Ngas, Nhengatu, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sisaali, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
-    </r>
-  </si>
-  <si>
     <t>The Salvation Story</t>
   </si>
   <si>
@@ -6342,12 +6320,15 @@
       <t>Themne,</t>
     </r>
   </si>
+  <si>
+    <t>Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, Bakhayo, Baniwa, Banjara, Bengali, Banyore, Bono, Bora, Buli, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Komo, Konkomba, Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lusamya, Luyole, Magogo, Marachi, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nawuri, Nchumburu, Ngas, Nhengatu, Ntrubo, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sekpele, Selee, Sisaali, Sisaala_Tumulung, Siwu, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuwuli, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6608,11 +6589,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -6659,7 +6635,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6742,6 +6718,9 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6752,7 +6731,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7248,13 +7227,13 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7426,12 +7405,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7576,12 +7555,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7899,12 +7878,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8036,12 +8015,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8650,12 +8629,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9195,12 +9174,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9496,12 +9475,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9741,12 +9720,12 @@
       <c r="A1" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>999</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10412,12 +10391,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>1019</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10602,12 +10581,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>1052</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10832,12 +10811,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11008,12 +10987,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>850</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11342,12 +11321,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11604,12 +11583,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11785,12 +11764,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12167,12 +12146,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12288,12 +12267,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>925</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12523,12 +12502,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>924</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12730,12 +12709,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12888,12 +12867,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>878</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13092,12 +13071,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13268,12 +13247,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -13471,12 +13450,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13646,12 +13625,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1107</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -13887,12 +13866,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1108</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -14134,12 +14113,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -23236,12 +23215,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1102</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -23377,12 +23356,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>1103</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -23508,8 +23487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23651,15 +23630,15 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="289" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A13" s="34" t="s">
         <v>812</v>
       </c>
       <c r="B13" s="41" t="s">
         <v>1199</v>
       </c>
-      <c r="C13" s="41" t="s">
-        <v>1252</v>
+      <c r="C13" s="51" t="s">
+        <v>1263</v>
       </c>
     </row>
   </sheetData>
@@ -23671,8 +23650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
   <dimension ref="A1:C211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72:C103"/>
+    <sheetView topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N111" sqref="N111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24427,19 +24406,19 @@
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="40" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="B70" s="40" t="s">
         <v>804</v>
       </c>
-      <c r="C70" s="50" t="s">
-        <v>1254</v>
+      <c r="C70" s="46" t="s">
+        <v>1253</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="40"/>
       <c r="B71" s="40"/>
-      <c r="C71" s="50"/>
+      <c r="C71" s="46"/>
     </row>
     <row r="72" spans="1:3" ht="187" x14ac:dyDescent="0.2">
       <c r="A72" s="42" t="s">
@@ -24449,7 +24428,7 @@
         <v>841</v>
       </c>
       <c r="C72" s="41" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24471,7 +24450,7 @@
         <v>841</v>
       </c>
       <c r="C74" s="41" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -24482,7 +24461,7 @@
         <v>841</v>
       </c>
       <c r="C75" s="41" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -24493,7 +24472,7 @@
         <v>841</v>
       </c>
       <c r="C76" s="41" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -24504,7 +24483,7 @@
         <v>841</v>
       </c>
       <c r="C77" s="41" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -24515,7 +24494,7 @@
         <v>841</v>
       </c>
       <c r="C78" s="41" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24526,7 +24505,7 @@
         <v>841</v>
       </c>
       <c r="C79" s="41" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24537,7 +24516,7 @@
         <v>841</v>
       </c>
       <c r="C80" s="41" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24548,7 +24527,7 @@
         <v>841</v>
       </c>
       <c r="C81" s="41" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24559,7 +24538,7 @@
         <v>841</v>
       </c>
       <c r="C82" s="41" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24570,7 +24549,7 @@
         <v>841</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24581,7 +24560,7 @@
         <v>841</v>
       </c>
       <c r="C84" s="41" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24592,7 +24571,7 @@
         <v>841</v>
       </c>
       <c r="C85" s="41" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24603,7 +24582,7 @@
         <v>841</v>
       </c>
       <c r="C86" s="41" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24614,7 +24593,7 @@
         <v>841</v>
       </c>
       <c r="C87" s="41" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24625,7 +24604,7 @@
         <v>841</v>
       </c>
       <c r="C88" s="41" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24636,7 +24615,7 @@
         <v>841</v>
       </c>
       <c r="C89" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24647,7 +24626,7 @@
         <v>841</v>
       </c>
       <c r="C90" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24658,7 +24637,7 @@
         <v>841</v>
       </c>
       <c r="C91" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24669,7 +24648,7 @@
         <v>841</v>
       </c>
       <c r="C92" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24680,7 +24659,7 @@
         <v>841</v>
       </c>
       <c r="C93" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24691,7 +24670,7 @@
         <v>841</v>
       </c>
       <c r="C94" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24702,7 +24681,7 @@
         <v>841</v>
       </c>
       <c r="C95" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24713,7 +24692,7 @@
         <v>841</v>
       </c>
       <c r="C96" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24724,7 +24703,7 @@
         <v>841</v>
       </c>
       <c r="C97" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24735,7 +24714,7 @@
         <v>841</v>
       </c>
       <c r="C98" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24746,7 +24725,7 @@
         <v>841</v>
       </c>
       <c r="C99" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24757,7 +24736,7 @@
         <v>841</v>
       </c>
       <c r="C100" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -24768,7 +24747,7 @@
         <v>841</v>
       </c>
       <c r="C101" s="41" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -24790,7 +24769,7 @@
         <v>841</v>
       </c>
       <c r="C103" s="41" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -26075,12 +26054,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>704</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -26508,12 +26487,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="48" t="s">
         <v>1171</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -26694,12 +26673,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>856</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -26892,12 +26871,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>889</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27065,12 +27044,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1241</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27240,12 +27219,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">

</xml_diff>

<commit_message>
Updating with new south africa campaign
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MicroDrive/SparrowGIT/TBM_Organization_Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8BE4BA-EDB9-AD4E-A7D9-EDF1A0CF4E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A51B2A-C3D0-B843-9AC7-8A903A986D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="21" activeTab="36" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="21" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -40,30 +40,31 @@
     <sheet name="TBMQN" sheetId="42" r:id="rId25"/>
     <sheet name="TBMQS" sheetId="25" r:id="rId26"/>
     <sheet name="TBMSA" sheetId="31" r:id="rId27"/>
-    <sheet name="TBMSL" sheetId="40" r:id="rId28"/>
-    <sheet name="Go_Build_Love" sheetId="17" r:id="rId29"/>
-    <sheet name="Kingdom_Ventures(Disabled)" sheetId="30" r:id="rId30"/>
-    <sheet name="KVMT" sheetId="47" r:id="rId31"/>
-    <sheet name="KVMR" sheetId="48" r:id="rId32"/>
-    <sheet name="Serve_Hope" sheetId="21" r:id="rId33"/>
-    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId34"/>
-    <sheet name="IPMRP" sheetId="45" r:id="rId35"/>
-    <sheet name="IPMRN" sheetId="46" r:id="rId36"/>
-    <sheet name="Wifi_Materials" sheetId="37" r:id="rId37"/>
-    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId38"/>
-    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId39"/>
-    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId40"/>
+    <sheet name="TBMSM" sheetId="51" r:id="rId28"/>
+    <sheet name="TBMSL" sheetId="40" r:id="rId29"/>
+    <sheet name="Go_Build_Love" sheetId="17" r:id="rId30"/>
+    <sheet name="Kingdom_Ventures(Disabled)" sheetId="30" r:id="rId31"/>
+    <sheet name="KVMT" sheetId="47" r:id="rId32"/>
+    <sheet name="KVMR" sheetId="48" r:id="rId33"/>
+    <sheet name="Serve_Hope" sheetId="21" r:id="rId34"/>
+    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId35"/>
+    <sheet name="IPMRP" sheetId="45" r:id="rId36"/>
+    <sheet name="IPMRN" sheetId="46" r:id="rId37"/>
+    <sheet name="Wifi_Materials" sheetId="37" r:id="rId38"/>
+    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId39"/>
+    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId40"/>
+    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId41"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId41"/>
+    <externalReference r:id="rId42"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="33" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
-    <definedName name="Reserved" localSheetId="28">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="34" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
     <definedName name="Reserved" localSheetId="29">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="31">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="30">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="32">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="31">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="33">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="0">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="1">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="2">[1]!tblReserved[Reserved keywords]</definedName>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4792" uniqueCount="1264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4821" uniqueCount="1273">
   <si>
     <t>Latitude</t>
   </si>
@@ -6323,6 +6324,33 @@
   <si>
     <t>Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, Bakhayo, Baniwa, Banjara, Bengali, Banyore, Bono, Bora, Buli, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Komo, Konkomba, Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lusamya, Luyole, Magogo, Marachi, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nawuri, Nchumburu, Ngas, Nhengatu, Ntrubo, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sekpele, Selee, Sisaali, Sisaala_Tumulung, Siwu, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuwuli, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
   </si>
+  <si>
+    <t>The Bucket Ministry South Africa - Mkholombe</t>
+  </si>
+  <si>
+    <t>Mkholombe - Sayitsini</t>
+  </si>
+  <si>
+    <t>Mkholombe - Mzakhele</t>
+  </si>
+  <si>
+    <t>Mkholombe - Marasta</t>
+  </si>
+  <si>
+    <t>Mkholombe - Emakhalibhothini</t>
+  </si>
+  <si>
+    <t>Mkholombe - Zone 14</t>
+  </si>
+  <si>
+    <t>Mkholombe - Nkopolo</t>
+  </si>
+  <si>
+    <t>Mkholombe - Ebhasini</t>
+  </si>
+  <si>
+    <t>Mkholombe - Bhoboyi</t>
+  </si>
 </sst>
 </file>
 
@@ -6635,7 +6663,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6721,6 +6749,10 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6732,7 +6764,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -6751,7 +6783,17 @@
     <cellStyle name="Normal 3 4 2" xfId="12" xr:uid="{3DEC3C28-17B5-4A3F-91B5-B6EF8513FB54}"/>
     <cellStyle name="Normal 3 5" xfId="8" xr:uid="{50844260-08FF-46B0-B10D-4A4539C5FF24}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7227,13 +7269,13 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7405,12 +7447,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7555,12 +7597,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7878,12 +7920,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8015,12 +8057,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8629,12 +8671,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9174,12 +9216,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9475,12 +9517,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9720,12 +9762,12 @@
       <c r="A1" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>999</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10391,12 +10433,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>1019</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10581,12 +10623,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>1052</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10811,12 +10853,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10987,12 +11029,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>850</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11321,12 +11363,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11583,12 +11625,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11764,12 +11806,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12146,12 +12188,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12267,12 +12309,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>925</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12502,12 +12544,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>924</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12709,12 +12751,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12830,7 +12872,7 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D13">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -12849,6 +12891,175 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B97DF68-E0AC-2F4E-A743-D3C1DDC3BEC7}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="47"/>
+    <col min="4" max="4" width="15" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="47"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="53" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>485</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="53" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>490</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="53" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="47" t="s">
+        <v>493</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="53" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="47" t="s">
+        <v>495</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="53" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="8" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="47" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="47" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D10" s="40"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" s="40"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D3:D13">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99931E6A-28C6-1147-AA7B-6F795C294FD1}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
   <dimension ref="A1:E18"/>
   <sheetViews>
@@ -12867,12 +13078,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>878</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13045,182 +13256,6 @@
             <xm:f>Validation!$B$1:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E5 E8:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E24D227-6B92-4869-A6EE-2CD0CE718ADB}">
-  <dimension ref="A1:E27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>391</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="D4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="D5" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="D6" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="D7" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="D8" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="3"/>
-      <c r="D9" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{782CE502-ED7E-4254-B847-1072C8C3A069}">
-          <x14:formula1>
-            <xm:f>Validation!$B$1:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -13247,12 +13282,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -13433,6 +13468,182 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E24D227-6B92-4869-A6EE-2CD0CE718ADB}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2"/>
+      <c r="D6" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+      <c r="D7" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="D8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{782CE502-ED7E-4254-B847-1072C8C3A069}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E0DFFC-07E8-40BE-8CA3-81702524BE9F}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -13450,12 +13661,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13607,7 +13818,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B04EE-2E1F-4050-B34E-0DBBEA1DCE38}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -13625,12 +13836,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1107</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -13848,7 +14059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79F542E-5CE0-43CC-9469-549164091111}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -13866,12 +14077,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1108</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -14094,7 +14305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8966E3F0-5F1C-45DE-88BD-0792C7795602}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -14113,12 +14324,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -14270,7 +14481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}">
   <dimension ref="A1:D636"/>
   <sheetViews>
@@ -23198,7 +23409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902D9A4C-CB6C-496C-ACF1-A89C91AD596C}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -23215,12 +23426,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1102</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -23339,7 +23550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE12B2DA-285C-4280-B25B-5772326A0B3F}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -23356,12 +23567,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1103</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -23483,11 +23694,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -23637,7 +23848,7 @@
       <c r="B13" s="41" t="s">
         <v>1199</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="48" t="s">
         <v>1263</v>
       </c>
     </row>
@@ -23646,7 +23857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
   <dimension ref="A1:C211"/>
   <sheetViews>
@@ -25962,73 +26173,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A72:A178">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:A205">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206:A211">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>414</v>
-      </c>
-      <c r="B1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>439</v>
-      </c>
-      <c r="B2" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>417</v>
-      </c>
-      <c r="B3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>480</v>
-      </c>
-      <c r="B4" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>441</v>
-      </c>
-      <c r="B5" t="s">
-        <v>482</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -26054,12 +26206,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>704</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -26320,6 +26472,65 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>417</v>
+      </c>
+      <c r="B3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>480</v>
+      </c>
+      <c r="B4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>441</v>
+      </c>
+      <c r="B5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -26487,12 +26698,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>1171</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -26673,12 +26884,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>856</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -26871,12 +27082,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>889</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27044,12 +27255,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="52" t="s">
         <v>1241</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27219,12 +27430,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">

</xml_diff>

<commit_message>
Updating Village Names and Org Name to follow the convention of the rest of the projects
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MicroDrive/SparrowGIT/TBM_Organization_Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A51B2A-C3D0-B843-9AC7-8A903A986D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FAC885-196A-9349-839E-2AB16BDA061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="21" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6325,31 +6325,31 @@
     <t>Afenmai, Ake-Levbu, Akoko, Akwai, Akyem, Amo, Anaguta, Ankwe, Annang, Bagim, Bajju, Bakhayo, Baniwa, Banjara, Bengali, Banyore, Bono, Bora, Buli, Bwai, Calabar, Chamba, Chawai, Chekosi, Chumburu, Creole, Criolo, Demark, Desano, Doemak, Edo, Efik, Eggon, Emai, Esan, Etsako, Etuno, Fante, Frafra, French, Fulfude (Fulani), Ga/Adangbe, Goemai, Gonja, Grune, Here, Hindi, Ibibio, Idoma, Igala, Igbanke, Igbo, Ijaw, Imua, Irigwe, Isoko, Itsekiri, Jarawa, Jukun, Kanjaga, Kannada, Kofia, Komo, Konkomba, Koro, Kotokoli, Krobo, Kulere, Kwal, Lemoro, Lubukusu, Lugwere, Lusamya, Luyole, Magogo, Marachi, Marathi, Marubo, Mernian, Minchika, Miranha, Miranhas, Mupun, Mura, Mushere, Mwaghavul, Nanuni, Nawuri, Nchumburu, Ngas, Nhengatu, Ntrubo, Ntu-Mbusor, Ogoja, Okpameri, Okpe, Oniyan, Oron, Other, Piraha, Piratapuyo, Pyem, Quan, Rindere, Ron, Rukuba (Bache), Satere-Mawe, Sekpele, Selee, Sisaali, Sisaala_Tumulung, Siwu, Skaryanas, Stiwa, Talni, Tamil, Tarok, Telugu, Tenharim, Ticuna, Tucano, Tula, Tuwuli, Tuyuca, Twi, Urhobo, Waali, Wamba, Wayway, Youm,</t>
   </si>
   <si>
-    <t>The Bucket Ministry South Africa - Mkholombe</t>
-  </si>
-  <si>
-    <t>Mkholombe - Sayitsini</t>
-  </si>
-  <si>
-    <t>Mkholombe - Mzakhele</t>
-  </si>
-  <si>
-    <t>Mkholombe - Marasta</t>
-  </si>
-  <si>
-    <t>Mkholombe - Emakhalibhothini</t>
-  </si>
-  <si>
-    <t>Mkholombe - Zone 14</t>
-  </si>
-  <si>
-    <t>Mkholombe - Nkopolo</t>
-  </si>
-  <si>
-    <t>Mkholombe - Ebhasini</t>
-  </si>
-  <si>
-    <t>Mkholombe - Bhoboyi</t>
+    <t>The Bucket Ministry Mkholombe</t>
+  </si>
+  <si>
+    <t>Sayitsini</t>
+  </si>
+  <si>
+    <t>Mzakhele</t>
+  </si>
+  <si>
+    <t>Marasta</t>
+  </si>
+  <si>
+    <t>Emakhalibhothini</t>
+  </si>
+  <si>
+    <t>Zone 14</t>
+  </si>
+  <si>
+    <t>Nkopolo</t>
+  </si>
+  <si>
+    <t>Ebhasini</t>
+  </si>
+  <si>
+    <t>Bhoboyi</t>
   </si>
 </sst>
 </file>
@@ -6753,6 +6753,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -6762,9 +6765,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -7269,13 +7269,13 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7447,12 +7447,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7597,12 +7597,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7920,12 +7920,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8057,12 +8057,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8671,12 +8671,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9216,12 +9216,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9517,12 +9517,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9762,12 +9762,12 @@
       <c r="A1" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>999</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10433,12 +10433,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>1019</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10623,12 +10623,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>1052</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -10853,12 +10853,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11029,12 +11029,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>850</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11363,12 +11363,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11625,12 +11625,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11806,12 +11806,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12188,12 +12188,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>406</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12309,12 +12309,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>925</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12544,12 +12544,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>924</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12751,12 +12751,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12895,7 +12895,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12911,12 +12911,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1264</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12936,7 +12936,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="49" t="s">
         <v>1265</v>
       </c>
       <c r="B3" s="47" t="s">
@@ -12953,7 +12953,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="49" t="s">
         <v>1266</v>
       </c>
       <c r="B4" s="3"/>
@@ -12968,7 +12968,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="49" t="s">
         <v>1267</v>
       </c>
       <c r="B5" s="3"/>
@@ -12983,7 +12983,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="49" t="s">
         <v>1268</v>
       </c>
       <c r="B6" s="2"/>
@@ -12998,7 +12998,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="49" t="s">
         <v>1269</v>
       </c>
       <c r="B7" s="3"/>
@@ -13041,7 +13041,7 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D13">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -13078,12 +13078,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>878</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13282,12 +13282,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -13486,12 +13486,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13661,12 +13661,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -13836,12 +13836,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1107</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -14077,12 +14077,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1108</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -14324,12 +14324,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -23426,12 +23426,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1102</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -23567,12 +23567,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>1103</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -26173,13 +26173,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A72:A178">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72:A205">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A206:A211">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26206,12 +26206,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>704</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -26698,12 +26698,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>1171</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
       <c r="F1" s="19" t="s">
         <v>496</v>
       </c>
@@ -26884,12 +26884,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>856</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27082,12 +27082,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>889</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27255,12 +27255,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>1241</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27430,12 +27430,12 @@
       <c r="A1" s="19" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -27594,14 +27594,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -27854,7 +27846,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -27863,24 +27855,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27899,10 +27882,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating with Original house and KVAR campaigns
</commit_message>
<xml_diff>
--- a/TBM Organization Parameters.xlsx
+++ b/TBM Organization Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MicroDrive/SparrowGIT/TBM_Organization_Parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B000E14A-87B4-AC47-9C9A-2DD1E29E7ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{C91E8DA0-4003-1C4F-8298-E14445E5B480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" tabRatio="813" firstSheet="18" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TBM" sheetId="7" r:id="rId1"/>
@@ -25,62 +25,65 @@
     <sheet name="TBMFI" sheetId="24" r:id="rId10"/>
     <sheet name="TBMG" sheetId="26" r:id="rId11"/>
     <sheet name="TBMI" sheetId="27" r:id="rId12"/>
-    <sheet name="TBMNJ" sheetId="11" r:id="rId13"/>
-    <sheet name="TBMKA" sheetId="5" r:id="rId14"/>
-    <sheet name="TBMK" sheetId="4" r:id="rId15"/>
-    <sheet name="TBMKI" sheetId="10" r:id="rId16"/>
-    <sheet name="TBMKS" sheetId="35" r:id="rId17"/>
-    <sheet name="TBMKN" sheetId="43" r:id="rId18"/>
-    <sheet name="TBMSS" sheetId="44" r:id="rId19"/>
-    <sheet name="TBMM" sheetId="23" r:id="rId20"/>
-    <sheet name="TBMN" sheetId="28" r:id="rId21"/>
-    <sheet name="TBMNG" sheetId="29" r:id="rId22"/>
-    <sheet name="TBMGN" sheetId="6" r:id="rId23"/>
-    <sheet name="TBMGT" sheetId="32" r:id="rId24"/>
-    <sheet name="TBMQN" sheetId="42" r:id="rId25"/>
-    <sheet name="TBMQS" sheetId="25" r:id="rId26"/>
-    <sheet name="TBMSA" sheetId="31" r:id="rId27"/>
-    <sheet name="TBMBSJ" sheetId="51" r:id="rId28"/>
-    <sheet name="TBMSL" sheetId="40" r:id="rId29"/>
-    <sheet name="Go_Build_Love" sheetId="17" r:id="rId30"/>
-    <sheet name="Kingdom_Ventures(Disabled)" sheetId="30" r:id="rId31"/>
-    <sheet name="KVMT" sheetId="47" r:id="rId32"/>
-    <sheet name="KVMR" sheetId="48" r:id="rId33"/>
-    <sheet name="KVNR" sheetId="52" r:id="rId34"/>
-    <sheet name="Serve_Hope" sheetId="21" r:id="rId35"/>
-    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId36"/>
-    <sheet name="IPMRP" sheetId="45" r:id="rId37"/>
-    <sheet name="IPMRN" sheetId="46" r:id="rId38"/>
-    <sheet name="Wifi_Materials" sheetId="37" r:id="rId39"/>
-    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId40"/>
-    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId41"/>
-    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId42"/>
+    <sheet name="TBMBJL" sheetId="53" r:id="rId13"/>
+    <sheet name="TBMNJ" sheetId="11" r:id="rId14"/>
+    <sheet name="TBMKA" sheetId="5" r:id="rId15"/>
+    <sheet name="TBMK" sheetId="4" r:id="rId16"/>
+    <sheet name="TBMKI" sheetId="10" r:id="rId17"/>
+    <sheet name="TBMKS" sheetId="35" r:id="rId18"/>
+    <sheet name="TBMKN" sheetId="43" r:id="rId19"/>
+    <sheet name="TBMSS" sheetId="44" r:id="rId20"/>
+    <sheet name="TBMM" sheetId="23" r:id="rId21"/>
+    <sheet name="TBMN" sheetId="28" r:id="rId22"/>
+    <sheet name="TBMNG" sheetId="29" r:id="rId23"/>
+    <sheet name="TBMGN" sheetId="6" r:id="rId24"/>
+    <sheet name="TBMGT" sheetId="32" r:id="rId25"/>
+    <sheet name="TBMQN" sheetId="42" r:id="rId26"/>
+    <sheet name="TBMQS" sheetId="25" r:id="rId27"/>
+    <sheet name="TBMSA" sheetId="31" r:id="rId28"/>
+    <sheet name="TBMBSJ" sheetId="51" r:id="rId29"/>
+    <sheet name="TBMSL" sheetId="40" r:id="rId30"/>
+    <sheet name="Go_Build_Love" sheetId="17" r:id="rId31"/>
+    <sheet name="Kingdom_Ventures(Disabled)" sheetId="30" r:id="rId32"/>
+    <sheet name="KVAR" sheetId="54" r:id="rId33"/>
+    <sheet name="KVMT" sheetId="47" r:id="rId34"/>
+    <sheet name="KVMR" sheetId="48" r:id="rId35"/>
+    <sheet name="KVNR" sheetId="52" r:id="rId36"/>
+    <sheet name="Serve_Hope" sheetId="21" r:id="rId37"/>
+    <sheet name="WiFi_Languages" sheetId="33" state="hidden" r:id="rId38"/>
+    <sheet name="IPMRP" sheetId="45" r:id="rId39"/>
+    <sheet name="IPMRN" sheetId="46" r:id="rId40"/>
+    <sheet name="Wifi_Materials" sheetId="37" r:id="rId41"/>
+    <sheet name="Wifi_Downloads" sheetId="38" r:id="rId42"/>
+    <sheet name="Validation" sheetId="34" state="hidden" r:id="rId43"/>
+    <sheet name="Data Valid" sheetId="2" state="hidden" r:id="rId44"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId43"/>
+    <externalReference r:id="rId45"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="35" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
-    <definedName name="Reserved" localSheetId="29">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="37" hidden="1">WiFi_Languages!$A$1:$D$636</definedName>
     <definedName name="Reserved" localSheetId="30">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="32">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="31">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="34">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="33">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="34">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="35">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="36">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="0">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="1">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="2">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="7">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="8">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="10">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="22">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="23">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="14">[1]!tblReserved[Reserved keywords]</definedName>
+    <definedName name="Reserved" localSheetId="16">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved" localSheetId="13">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="15">[1]!tblReserved[Reserved keywords]</definedName>
-    <definedName name="Reserved" localSheetId="12">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Reserved">[1]!tblReserved[Reserved keywords]</definedName>
     <definedName name="Special">[1]types!$A$169:$A$177</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -97,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4828" uniqueCount="1270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4891" uniqueCount="1306">
   <si>
     <t>Latitude</t>
   </si>
@@ -3908,19 +3911,134 @@
   </si>
   <si>
     <t>Jenta Tudu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cabeceira </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boa Vista </t>
+  </si>
+  <si>
+    <t>Rio Branco</t>
+  </si>
+  <si>
+    <t>Italiano</t>
+  </si>
+  <si>
+    <t>The Bucket Ministry Janauaca Lake</t>
+  </si>
+  <si>
+    <t>Kingdom Ventures Amazon River</t>
+  </si>
+  <si>
+    <t>El Milagro</t>
+  </si>
+  <si>
+    <t>Astoria</t>
+  </si>
+  <si>
+    <t>Santa Clotilde</t>
+  </si>
+  <si>
+    <t>Centro Arenal</t>
+  </si>
+  <si>
+    <t>Independencia</t>
+  </si>
+  <si>
+    <t>Barrio Florido</t>
+  </si>
+  <si>
+    <t>Costa Nera</t>
+  </si>
+  <si>
+    <t>Picuru Yacu</t>
+  </si>
+  <si>
+    <t>Santa Clara – Zona 1</t>
+  </si>
+  <si>
+    <t>Santa Clara – Zona 2</t>
+  </si>
+  <si>
+    <t>Santa Clara – Zona 3</t>
+  </si>
+  <si>
+    <t>Santa María de Ojeal</t>
+  </si>
+  <si>
+    <t>Nuevo Perú (Indígena)</t>
+  </si>
+  <si>
+    <t>Santa Zulema</t>
+  </si>
+  <si>
+    <t>San Juan de Sinchicuy</t>
+  </si>
+  <si>
+    <t>San Juan de Huashalado</t>
+  </si>
+  <si>
+    <t>Cabo Victor Pantoja</t>
+  </si>
+  <si>
+    <t>Santa María de Fátima</t>
+  </si>
+  <si>
+    <t>Sinchicuy</t>
+  </si>
+  <si>
+    <t>Juan Velasco</t>
+  </si>
+  <si>
+    <t>Nueva Amazonía</t>
+  </si>
+  <si>
+    <t>San Pedro de Huashalado</t>
+  </si>
+  <si>
+    <t>San Rafael</t>
+  </si>
+  <si>
+    <t>Santa María de Fátima 2</t>
+  </si>
+  <si>
+    <t>Padre Isla</t>
+  </si>
+  <si>
+    <t>Carococha</t>
+  </si>
+  <si>
+    <t>Santa Martha</t>
+  </si>
+  <si>
+    <t>Nueva Jerusalén</t>
+  </si>
+  <si>
+    <t>2 de Mayo</t>
+  </si>
+  <si>
+    <t>Indiana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -4199,102 +4317,106 @@
   </borders>
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="16" fontId="29" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="16" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4304,7 +4426,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4800,13 +4922,13 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -4978,12 +5100,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -5128,12 +5250,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>395</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -5451,12 +5573,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -5570,10 +5692,137 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC3F0E9-659C-5043-911C-9FAA7881B708}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="48" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="48" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="47" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="48" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="48"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="48"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FC8AA127-5648-B540-9CEA-777D1A90FB7A}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4914AC-81CB-46C7-BD71-CF158ABA186A}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -5588,12 +5837,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>397</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -6183,7 +6432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5B793A-E672-42F0-B7CD-796F921CC77D}">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -6202,12 +6451,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -6711,7 +6960,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -6728,7 +6977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FCEA8E-D73A-4C32-A54F-932DBA63E3E9}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -6747,12 +6996,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7030,7 +7279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7D1E55-F368-41C4-B6DD-BDC21E354B8B}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -7048,12 +7297,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -7272,7 +7521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39F5EFB-4C75-4F45-95CF-B50496BF741C}">
   <dimension ref="A1:G123"/>
   <sheetViews>
@@ -7293,12 +7542,12 @@
       <c r="A1" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>998</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -7942,7 +8191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A72036BD-30F9-4694-8C78-9BF67137CB5D}">
   <dimension ref="A1:G13"/>
   <sheetViews>
@@ -7964,12 +8213,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>1018</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -8122,239 +8371,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{18C712E4-CE2E-4622-BE04-7D735DBC72E1}">
-          <x14:formula1>
-            <xm:f>Validation!$B$1:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E7</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513B32ED-D4ED-4AAF-9640-558CF71915D7}">
-  <dimension ref="A1:G21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="48" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="19" t="s">
-        <v>495</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>1049</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>1075</v>
-      </c>
-      <c r="E3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>1070</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1052</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>1071</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>1069</v>
-      </c>
-      <c r="E5" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1053</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>1072</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>1054</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>1073</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1055</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>1074</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1056</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1057</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>1058</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>1059</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>1060</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>1061</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>1062</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{519959BF-E3F8-48FA-9A5C-3649EC2B50A1}">
           <x14:formula1>
             <xm:f>Validation!$B$1:$B$5</xm:f>
           </x14:formula1>
@@ -8385,12 +8401,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>391</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8543,6 +8559,239 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{513B32ED-D4ED-4AAF-9640-558CF71915D7}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>1069</v>
+      </c>
+      <c r="E5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1055</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{519959BF-E3F8-48FA-9A5C-3649EC2B50A1}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA7208EC-C09B-46BC-9208-53E975DA3383}">
   <dimension ref="A1:E34"/>
   <sheetViews>
@@ -8561,12 +8810,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>849</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -8875,7 +9124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00598E5C-D8DC-4176-B37C-0365BB6BC78A}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -8895,12 +9144,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9137,7 +9386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14823A46-4501-4F96-80B3-10A0CC5D20D3}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9157,12 +9406,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>401</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9318,7 +9567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E969F7E-8CCE-43F9-9791-7FA2BD394061}">
   <dimension ref="A1:E30"/>
   <sheetViews>
@@ -9338,12 +9587,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>402</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9702,7 +9951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9796B9BC-A579-4EDE-99EB-40D54CC290A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -9720,12 +9969,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>405</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -9821,7 +10070,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E80414F-2A51-4046-8BC5-8F857B02E2CD}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -9841,12 +10090,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>924</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10056,7 +10305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0B993E-AFCD-4B7D-9D40-53D866792064}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -10076,12 +10325,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>923</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10264,7 +10513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748FCB8D-0FD0-4AE3-B979-7656B5CF254B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -10283,12 +10532,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>404</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10422,7 +10671,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C836D619-F1A1-794E-85C4-9575A5F159DC}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -10443,12 +10692,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1261</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -10536,210 +10785,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02549DA9-760F-314A-A016-BA38ED4F129F}">
-          <x14:formula1>
-            <xm:f>Validation!$B$1:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E3:E5 E8:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
-  <dimension ref="A1:E18"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>877</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="34" t="s">
-        <v>884</v>
-      </c>
-      <c r="C3" t="s">
-        <v>878</v>
-      </c>
-      <c r="D3" t="s">
-        <v>878</v>
-      </c>
-      <c r="E3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="34" t="s">
-        <v>883</v>
-      </c>
-      <c r="C4" t="s">
-        <v>879</v>
-      </c>
-      <c r="D4" t="s">
-        <v>879</v>
-      </c>
-      <c r="E4" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="34" t="s">
-        <v>885</v>
-      </c>
-      <c r="C5" t="s">
-        <v>880</v>
-      </c>
-      <c r="D5" t="s">
-        <v>880</v>
-      </c>
-      <c r="E5" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="34" t="s">
-        <v>886</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>881</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>881</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
-        <v>887</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>1190</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>1190</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>1101</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="40" t="s">
-        <v>1191</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>1191</v>
-      </c>
-      <c r="E8" s="40"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>907</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="40" t="s">
-        <v>1192</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>1192</v>
-      </c>
-      <c r="E9" s="40"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD20C374-E3CD-408E-8EB0-BA328822C0D2}">
           <x14:formula1>
             <xm:f>Validation!$B$1:$B$5</xm:f>
           </x14:formula1>
@@ -10770,12 +10815,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>392</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
@@ -10956,6 +11001,210 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4580856D-F3F7-4DE2-A933-D6C97E9CD1DE}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>877</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>884</v>
+      </c>
+      <c r="C3" t="s">
+        <v>878</v>
+      </c>
+      <c r="D3" t="s">
+        <v>878</v>
+      </c>
+      <c r="E3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>883</v>
+      </c>
+      <c r="C4" t="s">
+        <v>879</v>
+      </c>
+      <c r="D4" t="s">
+        <v>879</v>
+      </c>
+      <c r="E4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
+        <v>885</v>
+      </c>
+      <c r="C5" t="s">
+        <v>880</v>
+      </c>
+      <c r="D5" t="s">
+        <v>880</v>
+      </c>
+      <c r="E5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="34" t="s">
+        <v>886</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>881</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>881</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
+        <v>887</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="40" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>1191</v>
+      </c>
+      <c r="E8" s="40"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>907</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="40" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>1192</v>
+      </c>
+      <c r="E9" s="40"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DD20C374-E3CD-408E-8EB0-BA328822C0D2}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E3:E5 E8:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E24D227-6B92-4869-A6EE-2CD0CE718ADB}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -10974,12 +11223,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11131,7 +11380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E0DFFC-07E8-40BE-8CA3-81702524BE9F}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -11149,12 +11398,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>403</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -11306,7 +11555,268 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{101EB3AF-CB54-084C-83EA-DC897616F1CF}">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="27"/>
+      <c r="E4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="28"/>
+      <c r="E5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B6" s="31"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="48"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="48"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8DE09BA5-E1EE-1F40-A3A7-E4D517AF1066}">
+          <x14:formula1>
+            <xm:f>Validation!$B$1:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87B04EE-2E1F-4050-B34E-0DBBEA1DCE38}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -11324,12 +11834,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1104</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -11547,7 +12057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D79F542E-5CE0-43CC-9469-549164091111}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -11565,12 +12075,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1105</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -11793,7 +12303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02412546-1E56-064A-A0B9-8BC40AE3458E}">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -11811,12 +12321,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1263</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -11980,7 +12490,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8966E3F0-5F1C-45DE-88BD-0792C7795602}">
   <dimension ref="A1:E27"/>
   <sheetViews>
@@ -11999,12 +12509,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -12156,7 +12666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FB02A95-1B06-4367-B3E8-F4078367DB11}">
   <dimension ref="A1:D636"/>
   <sheetViews>
@@ -21084,7 +21594,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902D9A4C-CB6C-496C-ACF1-A89C91AD596C}">
   <dimension ref="A1:G15"/>
   <sheetViews>
@@ -21101,12 +21611,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>1099</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -21221,313 +21731,6 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE12B2DA-285C-4280-B25B-5772326A0B3F}">
-  <dimension ref="A1:G15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>390</v>
-      </c>
-      <c r="B1" s="47" t="s">
-        <v>1100</v>
-      </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="19" t="s">
-        <v>495</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1093</v>
-      </c>
-      <c r="B3" t="s">
-        <v>117</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1094</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="D4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>1095</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="D5" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1096</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="D6" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>1097</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1098</v>
-      </c>
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>1161</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="59.1640625" style="40" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
-        <v>798</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>804</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>799</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>1254</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>1244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="40" t="s">
-        <v>442</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>412</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>810</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>414</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>810</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>497</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>810</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>498</v>
-      </c>
-      <c r="B7" s="39" t="s">
-        <v>810</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="255" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>800</v>
-      </c>
-      <c r="B8" s="39" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
-        <v>801</v>
-      </c>
-      <c r="B9" s="39" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>479</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>1193</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>802</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>803</v>
-      </c>
-      <c r="B12" s="39" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>1242</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A13" s="39" t="s">
-        <v>811</v>
-      </c>
-      <c r="B13" s="39" t="s">
-        <v>1194</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>1243</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21553,12 +21756,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>703</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -21801,7 +22004,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -21819,6 +22022,313 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE12B2DA-285C-4280-B25B-5772326A0B3F}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="D5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4090C0-81F3-488A-BFE0-128FBADFA632}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.1640625" style="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="40" t="s">
+        <v>798</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>804</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>799</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>810</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>810</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>497</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>810</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
+        <v>498</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>810</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>800</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>801</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>479</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>802</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>803</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+      <c r="A13" s="39" t="s">
+        <v>811</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B17A051-E04F-4C5E-BBD2-8BC11DFBB7DE}">
   <dimension ref="A1:C211"/>
   <sheetViews>
@@ -24145,7 +24655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0388E7-6D7C-494A-B5B0-A06D9161366A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -24204,7 +24714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -24372,12 +24882,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="50" t="s">
         <v>1168</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
       <c r="F1" s="19" t="s">
         <v>495</v>
       </c>
@@ -24558,12 +25068,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>855</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -24756,12 +25266,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>888</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -24929,12 +25439,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="52" t="s">
         <v>1236</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -25104,12 +25614,12 @@
       <c r="A1" s="19" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
@@ -25268,14 +25778,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -25284,7 +25786,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D3C69E808006664F9CCA3D9BC71AC55D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5845cacad74656bcde11e00306ad31f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d75e0231-c5c8-4c84-8215-b760034bdfa5" xmlns:ns4="621de0e2-4b56-4c44-bb0f-ce9b0aec4994" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2cb8dbf20762a8ba415eee6dfba6bc92" ns3:_="" ns4:_="">
     <xsd:import namespace="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
@@ -25537,24 +26039,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d75e0231-c5c8-4c84-8215-b760034bdfa5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F41548EA-A522-4942-9ABF-935FDE65872B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -25562,7 +26055,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B426DB6-4B6A-4971-948B-870FFF62E8F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25579,4 +26072,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B09A22F1-B742-4DEC-998C-03DEA5FA7C76}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="621de0e2-4b56-4c44-bb0f-ce9b0aec4994"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="d75e0231-c5c8-4c84-8215-b760034bdfa5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>